<commit_message>
updated Web Apps 1
</commit_message>
<xml_diff>
--- a/CS320-Spring2018Calendar.xlsx
+++ b/CS320-Spring2018Calendar.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="73">
   <si>
     <t>Monday</t>
   </si>
@@ -127,14 +127,6 @@
 BD Guest Lecturer</t>
   </si>
   <si>
-    <t>Web Applications Exercise &amp; Lab 2
-(in class)</t>
-  </si>
-  <si>
-    <t>CS320: SW Engineering - Spring 2018 Schedule
-(as of 12-23-2018, subject to change)</t>
-  </si>
-  <si>
     <t>Lecture 7:
 Agile Development and Scrum</t>
   </si>
@@ -167,10 +159,6 @@
 (Marmoset)
 A11: Team Project
 Final Self/Peer Evaluations due
-(Marmoset)</t>
-  </si>
-  <si>
-    <t>Lab 2: Web Apps due
 (Marmoset)</t>
   </si>
   <si>
@@ -197,23 +185,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Lecture 4: Web Applications
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Lab 2: Web Applications assigned</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve">Lecture 13: Relational Databases
 </t>
     </r>
@@ -360,6 +331,39 @@
   <si>
     <t>A09: Individual Code &amp; Report due
 (Marmoset)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Lecture 4: Web Applications
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Lab 2a: Web Applications assigned</t>
+    </r>
+  </si>
+  <si>
+    <t>Lab 2a: Web Apps II due
+(Marmoset)</t>
+  </si>
+  <si>
+    <t>Lab 2: Web Apps I due
+(Marmoset)</t>
+  </si>
+  <si>
+    <t>Web Applications I Exercise &amp; Lab 2
+(in class)</t>
+  </si>
+  <si>
+    <t>CS320: SW Engineering - Spring 2018 Schedule
+(as of 1-16-2018, subject to change)</t>
   </si>
 </sst>
 </file>
@@ -931,7 +935,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="112">
+  <cellXfs count="113">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1191,31 +1195,43 @@
     <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1242,6 +1258,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
@@ -1251,19 +1270,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1572,8 +1579,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I52" sqref="I52"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1591,21 +1598,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="57.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="91" t="s">
-        <v>31</v>
-      </c>
-      <c r="B1" s="92"/>
-      <c r="C1" s="92"/>
-      <c r="D1" s="92"/>
-      <c r="E1" s="92"/>
-      <c r="F1" s="92"/>
-      <c r="G1" s="92"/>
-      <c r="H1" s="92"/>
-      <c r="I1" s="93"/>
+      <c r="A1" s="94" t="s">
+        <v>72</v>
+      </c>
+      <c r="B1" s="95"/>
+      <c r="C1" s="95"/>
+      <c r="D1" s="95"/>
+      <c r="E1" s="95"/>
+      <c r="F1" s="95"/>
+      <c r="G1" s="95"/>
+      <c r="H1" s="95"/>
+      <c r="I1" s="96"/>
     </row>
     <row r="2" spans="1:13" s="2" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1" t="s">
@@ -1631,10 +1638,10 @@
       </c>
     </row>
     <row r="3" spans="1:13" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="94">
+      <c r="A3" s="99">
         <v>16</v>
       </c>
-      <c r="B3" s="98" t="s">
+      <c r="B3" s="102" t="s">
         <v>14</v>
       </c>
       <c r="C3" s="66">
@@ -1666,8 +1673,8 @@
       </c>
     </row>
     <row r="4" spans="1:13" ht="81.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="87"/>
-      <c r="B4" s="99"/>
+      <c r="A4" s="92"/>
+      <c r="B4" s="103"/>
       <c r="C4" s="64" t="s">
         <v>11</v>
       </c>
@@ -1678,19 +1685,19 @@
         <v>11</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="G4" s="8"/>
       <c r="H4" s="7" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="I4" s="9"/>
     </row>
     <row r="5" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="87">
+      <c r="A5" s="92">
         <v>15</v>
       </c>
-      <c r="B5" s="99"/>
+      <c r="B5" s="103"/>
       <c r="C5" s="10">
         <f>I3 + 1</f>
         <v>21</v>
@@ -1721,29 +1728,31 @@
       </c>
     </row>
     <row r="6" spans="1:13" ht="82.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="87"/>
-      <c r="B6" s="99"/>
+      <c r="A6" s="92"/>
+      <c r="B6" s="103"/>
       <c r="C6" s="63" t="s">
         <v>10</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>43</v>
+        <v>68</v>
       </c>
       <c r="E6" s="8"/>
       <c r="F6" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="G6" s="8"/>
+        <v>71</v>
+      </c>
+      <c r="G6" s="61" t="s">
+        <v>70</v>
+      </c>
       <c r="H6" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="I6" s="9"/>
+        <v>50</v>
+      </c>
+      <c r="I6" s="112"/>
     </row>
     <row r="7" spans="1:13" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="87">
+      <c r="A7" s="92">
         <v>14</v>
       </c>
-      <c r="B7" s="99"/>
+      <c r="B7" s="103"/>
       <c r="C7" s="10">
         <f>I5 + 1</f>
         <v>28</v>
@@ -1768,18 +1777,18 @@
         <v>2</v>
       </c>
       <c r="I7" s="13">
-        <f>H7 + 1</f>
+        <f>H7+1</f>
         <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="88"/>
-      <c r="B8" s="100"/>
-      <c r="C8" s="110" t="s">
+      <c r="A8" s="93"/>
+      <c r="B8" s="104"/>
+      <c r="C8" s="90" t="s">
         <v>21</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E8" s="30"/>
       <c r="F8" s="55" t="s">
@@ -1787,17 +1796,17 @@
       </c>
       <c r="G8" s="17"/>
       <c r="H8" s="16" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="I8" s="62" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="94">
+      <c r="A9" s="99">
         <v>13</v>
       </c>
-      <c r="B9" s="101" t="s">
+      <c r="B9" s="105" t="s">
         <v>15</v>
       </c>
       <c r="C9" s="20">
@@ -1830,29 +1839,29 @@
       </c>
     </row>
     <row r="10" spans="1:13" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="87"/>
-      <c r="B10" s="102"/>
+      <c r="A10" s="92"/>
+      <c r="B10" s="106"/>
       <c r="C10" s="63" t="s">
-        <v>40</v>
+        <v>69</v>
       </c>
       <c r="D10" s="18" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E10" s="17"/>
       <c r="F10" s="18" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="G10" s="17"/>
       <c r="H10" s="18" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="I10" s="19"/>
     </row>
     <row r="11" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="87">
+      <c r="A11" s="92">
         <v>12</v>
       </c>
-      <c r="B11" s="102"/>
+      <c r="B11" s="106"/>
       <c r="C11" s="24">
         <f>I9 + 1</f>
         <v>11</v>
@@ -1883,17 +1892,17 @@
       </c>
     </row>
     <row r="12" spans="1:13" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="87"/>
-      <c r="B12" s="102"/>
+      <c r="A12" s="92"/>
+      <c r="B12" s="106"/>
       <c r="C12" s="63" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D12" s="18" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E12" s="17"/>
       <c r="F12" s="18" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="G12" s="17"/>
       <c r="H12" s="18" t="s">
@@ -1902,10 +1911,10 @@
       <c r="I12" s="19"/>
     </row>
     <row r="13" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="87">
+      <c r="A13" s="92">
         <v>11</v>
       </c>
-      <c r="B13" s="102"/>
+      <c r="B13" s="106"/>
       <c r="C13" s="24">
         <f>I11 + 1</f>
         <v>18</v>
@@ -1936,19 +1945,19 @@
       </c>
     </row>
     <row r="14" spans="1:13" ht="83.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="87"/>
-      <c r="B14" s="102"/>
+      <c r="A14" s="92"/>
+      <c r="B14" s="106"/>
       <c r="C14" s="24"/>
       <c r="D14" s="18" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E14" s="17"/>
       <c r="F14" s="51" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G14" s="16"/>
       <c r="H14" s="18" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="I14" s="62" t="s">
         <v>9</v>
@@ -1957,10 +1966,10 @@
       <c r="M14" s="42"/>
     </row>
     <row r="15" spans="1:13" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="87">
+      <c r="A15" s="92">
         <v>10</v>
       </c>
-      <c r="B15" s="102"/>
+      <c r="B15" s="106"/>
       <c r="C15" s="64">
         <f>I13 + 1</f>
         <v>25</v>
@@ -1990,10 +1999,10 @@
       </c>
     </row>
     <row r="16" spans="1:13" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="88"/>
-      <c r="B16" s="103"/>
+      <c r="A16" s="93"/>
+      <c r="B16" s="107"/>
       <c r="C16" s="71" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D16" s="72" t="str">
         <f t="shared" ref="D16:I16" si="2">C16</f>
@@ -2035,8 +2044,8 @@
       <c r="A18" s="81"/>
       <c r="B18" s="35"/>
       <c r="D18" s="38"/>
-      <c r="E18" s="111" t="s">
-        <v>58</v>
+      <c r="E18" s="91" t="s">
+        <v>54</v>
       </c>
       <c r="F18" s="38"/>
       <c r="G18" s="38"/>
@@ -2048,7 +2057,7 @@
       <c r="B19" s="40"/>
       <c r="D19" s="34"/>
       <c r="E19" s="82" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="F19" s="34"/>
       <c r="G19" s="34"/>
@@ -2060,7 +2069,7 @@
       <c r="B20" s="35"/>
       <c r="D20" s="38"/>
       <c r="E20" s="83" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="F20" s="38"/>
       <c r="G20" s="38"/>
@@ -2072,7 +2081,7 @@
       <c r="B21" s="35"/>
       <c r="D21" s="38"/>
       <c r="E21" s="84" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="F21" s="38"/>
       <c r="G21" s="38"/>
@@ -2084,7 +2093,7 @@
       <c r="B22" s="35"/>
       <c r="D22" s="38"/>
       <c r="E22" s="85" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="F22" s="38"/>
       <c r="G22" s="38"/>
@@ -2097,7 +2106,7 @@
       <c r="C23" s="80"/>
       <c r="D23" s="38"/>
       <c r="E23" s="86" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="F23" s="38"/>
       <c r="G23" s="38"/>
@@ -2138,19 +2147,19 @@
       <c r="I26" s="38"/>
     </row>
     <row r="27" spans="1:11" s="36" customFormat="1" ht="57.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="91" t="str">
+      <c r="A27" s="94" t="str">
         <f>A1</f>
         <v>CS320: SW Engineering - Spring 2018 Schedule
-(as of 12-23-2018, subject to change)</v>
-      </c>
-      <c r="B27" s="92"/>
-      <c r="C27" s="92"/>
-      <c r="D27" s="92"/>
-      <c r="E27" s="92"/>
-      <c r="F27" s="92"/>
-      <c r="G27" s="92"/>
-      <c r="H27" s="92"/>
-      <c r="I27" s="93"/>
+(as of 1-16-2018, subject to change)</v>
+      </c>
+      <c r="B27" s="95"/>
+      <c r="C27" s="95"/>
+      <c r="D27" s="95"/>
+      <c r="E27" s="95"/>
+      <c r="F27" s="95"/>
+      <c r="G27" s="95"/>
+      <c r="H27" s="95"/>
+      <c r="I27" s="96"/>
     </row>
     <row r="28" spans="1:11" s="2" customFormat="1" ht="17.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="str">
@@ -2191,11 +2200,11 @@
       </c>
     </row>
     <row r="29" spans="1:11" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="95">
+      <c r="A29" s="97">
         <v>10</v>
       </c>
-      <c r="B29" s="96" t="s">
-        <v>50</v>
+      <c r="B29" s="100" t="s">
+        <v>46</v>
       </c>
       <c r="C29" s="64">
         <f>C15</f>
@@ -2226,10 +2235,10 @@
       </c>
     </row>
     <row r="30" spans="1:11" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="90"/>
-      <c r="B30" s="97"/>
+      <c r="A30" s="98"/>
+      <c r="B30" s="101"/>
       <c r="C30" s="77" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D30" s="75" t="str">
         <f t="shared" ref="D30" si="5">C30</f>
@@ -2257,10 +2266,10 @@
       </c>
     </row>
     <row r="31" spans="1:11" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="94">
+      <c r="A31" s="99">
         <v>9</v>
       </c>
-      <c r="B31" s="98" t="s">
+      <c r="B31" s="102" t="s">
         <v>16</v>
       </c>
       <c r="C31" s="64">
@@ -2293,24 +2302,24 @@
       </c>
     </row>
     <row r="32" spans="1:11" ht="86.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="87"/>
-      <c r="B32" s="99"/>
+      <c r="A32" s="92"/>
+      <c r="B32" s="103"/>
       <c r="C32" s="64" t="str">
         <f>I30</f>
         <v>WINTER BREAK</v>
       </c>
       <c r="D32" s="27" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="E32" s="61" t="s">
         <v>25</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="G32" s="7"/>
       <c r="H32" s="7" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="I32" s="61" t="s">
         <v>24</v>
@@ -2318,10 +2327,10 @@
       <c r="K32" s="43"/>
     </row>
     <row r="33" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="87">
+      <c r="A33" s="92">
         <v>8</v>
       </c>
-      <c r="B33" s="99"/>
+      <c r="B33" s="103"/>
       <c r="C33" s="28">
         <f>I31 + 1</f>
         <v>11</v>
@@ -2352,19 +2361,19 @@
       </c>
     </row>
     <row r="34" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="87"/>
-      <c r="B34" s="99"/>
+      <c r="A34" s="92"/>
+      <c r="B34" s="103"/>
       <c r="C34" s="10"/>
       <c r="D34" s="45" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="E34" s="7"/>
       <c r="F34" s="7" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="G34" s="7"/>
       <c r="H34" s="7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="I34" s="62" t="s">
         <v>26</v>
@@ -2372,10 +2381,10 @@
       <c r="K34" s="41"/>
     </row>
     <row r="35" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="87">
+      <c r="A35" s="92">
         <v>7</v>
       </c>
-      <c r="B35" s="99"/>
+      <c r="B35" s="103"/>
       <c r="C35" s="10">
         <f>I33 + 1</f>
         <v>18</v>
@@ -2406,15 +2415,15 @@
       </c>
     </row>
     <row r="36" spans="1:11" ht="54" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="87"/>
-      <c r="B36" s="99"/>
+      <c r="A36" s="92"/>
+      <c r="B36" s="103"/>
       <c r="C36" s="10"/>
       <c r="D36" s="32" t="s">
         <v>19</v>
       </c>
       <c r="E36" s="8"/>
       <c r="F36" s="7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G36" s="7"/>
       <c r="H36" s="7" t="s">
@@ -2423,10 +2432,10 @@
       <c r="I36" s="11"/>
     </row>
     <row r="37" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="87">
+      <c r="A37" s="92">
         <v>6</v>
       </c>
-      <c r="B37" s="99"/>
+      <c r="B37" s="103"/>
       <c r="C37" s="10">
         <f>I35 + 1</f>
         <v>25</v>
@@ -2457,11 +2466,11 @@
       </c>
     </row>
     <row r="38" spans="1:11" ht="44.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="88"/>
-      <c r="B38" s="100"/>
+      <c r="A38" s="93"/>
+      <c r="B38" s="104"/>
       <c r="C38" s="29"/>
       <c r="D38" s="44" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="E38" s="30"/>
       <c r="F38" s="56" t="s">
@@ -2478,10 +2487,10 @@
       </c>
     </row>
     <row r="39" spans="1:11" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="94">
+      <c r="A39" s="99">
         <v>5</v>
       </c>
-      <c r="B39" s="104" t="s">
+      <c r="B39" s="109" t="s">
         <v>17</v>
       </c>
       <c r="C39" s="64">
@@ -2513,8 +2522,8 @@
       </c>
     </row>
     <row r="40" spans="1:11" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="87"/>
-      <c r="B40" s="105"/>
+      <c r="A40" s="92"/>
+      <c r="B40" s="110"/>
       <c r="C40" s="64" t="s">
         <v>7</v>
       </c>
@@ -2526,18 +2535,18 @@
         <v>8</v>
       </c>
       <c r="G40" s="17"/>
-      <c r="H40" s="108" t="s">
-        <v>59</v>
+      <c r="H40" s="88" t="s">
+        <v>55</v>
       </c>
       <c r="I40" s="62" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="41" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="87">
+      <c r="A41" s="92">
         <v>4</v>
       </c>
-      <c r="B41" s="105"/>
+      <c r="B41" s="110"/>
       <c r="C41" s="24">
         <f>I39 + 1</f>
         <v>8</v>
@@ -2568,11 +2577,11 @@
       </c>
     </row>
     <row r="42" spans="1:11" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="87"/>
-      <c r="B42" s="105"/>
-      <c r="C42" s="107"/>
+      <c r="A42" s="92"/>
+      <c r="B42" s="110"/>
+      <c r="C42" s="87"/>
       <c r="D42" s="45" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="E42" s="17"/>
       <c r="F42" s="31" t="s">
@@ -2585,10 +2594,10 @@
       <c r="I42" s="54"/>
     </row>
     <row r="43" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="87">
+      <c r="A43" s="92">
         <v>3</v>
       </c>
-      <c r="B43" s="105"/>
+      <c r="B43" s="110"/>
       <c r="C43" s="59">
         <f>I41 + 1</f>
         <v>15</v>
@@ -2619,11 +2628,11 @@
       </c>
     </row>
     <row r="44" spans="1:11" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="87"/>
-      <c r="B44" s="105"/>
+      <c r="A44" s="92"/>
+      <c r="B44" s="110"/>
       <c r="C44" s="57"/>
       <c r="D44" s="32" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="E44" s="17"/>
       <c r="F44" s="31" t="s">
@@ -2636,10 +2645,10 @@
       <c r="I44" s="19"/>
     </row>
     <row r="45" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="87">
+      <c r="A45" s="92">
         <v>2</v>
       </c>
-      <c r="B45" s="105"/>
+      <c r="B45" s="110"/>
       <c r="C45" s="24">
         <f>I43 + 1</f>
         <v>22</v>
@@ -2670,14 +2679,14 @@
       </c>
     </row>
     <row r="46" spans="1:11" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="87"/>
-      <c r="B46" s="105"/>
+      <c r="A46" s="92"/>
+      <c r="B46" s="110"/>
       <c r="C46" s="23"/>
       <c r="D46" s="45" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="E46" s="61" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="F46" s="31" t="s">
         <v>8</v>
@@ -2689,11 +2698,11 @@
       <c r="I46" s="19"/>
     </row>
     <row r="47" spans="1:11" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="87">
+      <c r="A47" s="92">
         <f>A50 + 1</f>
         <v>1</v>
       </c>
-      <c r="B47" s="105"/>
+      <c r="B47" s="110"/>
       <c r="C47" s="24">
         <f>I45 + 1</f>
         <v>29</v>
@@ -2723,8 +2732,8 @@
       </c>
     </row>
     <row r="48" spans="1:11" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="88"/>
-      <c r="B48" s="106"/>
+      <c r="A48" s="93"/>
+      <c r="B48" s="111"/>
       <c r="C48" s="48"/>
       <c r="D48" s="58" t="s">
         <v>8</v>
@@ -2740,10 +2749,10 @@
       </c>
     </row>
     <row r="49" spans="1:9" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="89">
+      <c r="A49" s="108">
         <v>0</v>
       </c>
-      <c r="B49" s="98" t="s">
+      <c r="B49" s="102" t="s">
         <v>5</v>
       </c>
       <c r="C49" s="10">
@@ -2776,12 +2785,12 @@
       </c>
     </row>
     <row r="50" spans="1:9" ht="129.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="90"/>
-      <c r="B50" s="100"/>
+      <c r="A50" s="98"/>
+      <c r="B50" s="104"/>
       <c r="C50" s="14"/>
       <c r="D50" s="14"/>
-      <c r="E50" s="109" t="s">
-        <v>39</v>
+      <c r="E50" s="89" t="s">
+        <v>37</v>
       </c>
       <c r="F50" s="33" t="s">
         <v>28</v>
@@ -2793,6 +2802,18 @@
     <row r="51" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="A47:A48"/>
+    <mergeCell ref="A49:A50"/>
+    <mergeCell ref="A27:I27"/>
+    <mergeCell ref="A33:A34"/>
+    <mergeCell ref="A35:A36"/>
+    <mergeCell ref="A37:A38"/>
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="A41:A42"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="B39:B48"/>
     <mergeCell ref="A13:A14"/>
     <mergeCell ref="A15:A16"/>
     <mergeCell ref="A1:I1"/>
@@ -2807,18 +2828,6 @@
     <mergeCell ref="B31:B38"/>
     <mergeCell ref="B3:B8"/>
     <mergeCell ref="B9:B16"/>
-    <mergeCell ref="A43:A44"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="A47:A48"/>
-    <mergeCell ref="A49:A50"/>
-    <mergeCell ref="A27:I27"/>
-    <mergeCell ref="A33:A34"/>
-    <mergeCell ref="A35:A36"/>
-    <mergeCell ref="A37:A38"/>
-    <mergeCell ref="A39:A40"/>
-    <mergeCell ref="A41:A42"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="B39:B48"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="5" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
updated for scrum lecture
</commit_message>
<xml_diff>
--- a/CS320-Spring2018Calendar.xlsx
+++ b/CS320-Spring2018Calendar.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\djhake2\cs320-spring2018\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="90" yWindow="-165" windowWidth="15825" windowHeight="12075"/>
   </bookViews>
@@ -16,7 +11,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -126,10 +121,6 @@
 A08: Team Presentation and Demonstration
 (in class)
 </t>
-  </si>
-  <si>
-    <t>Lecture 7:
-Agile Development and Scrum</t>
   </si>
   <si>
     <t>Lecture 11: OO Design, OCP, LSP
@@ -363,13 +354,19 @@
 (in class)</t>
   </si>
   <si>
-    <t>CS320: SW Engineering - Spring 2018 Schedule
-(as of 1-26-2018, subject to change)</t>
-  </si>
-  <si>
     <t>Web Applications II
 (Lab 2a)
 (in class)</t>
+  </si>
+  <si>
+    <t>Lecture 7:
+Agile &amp; Scrum
+(Agile Manifesto)
+(Scrum Guide)</t>
+  </si>
+  <si>
+    <t>CS320: SW Engineering - Spring 2018 Schedule
+(as of 1-29-2018, subject to change)</t>
   </si>
 </sst>
 </file>
@@ -1225,30 +1222,51 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
@@ -1256,27 +1274,6 @@
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1339,7 +1336,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1374,7 +1371,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1586,7 +1583,7 @@
   <dimension ref="A1:M51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection sqref="A1:I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1604,21 +1601,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="57.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="97" t="s">
-        <v>71</v>
-      </c>
-      <c r="B1" s="98"/>
-      <c r="C1" s="98"/>
-      <c r="D1" s="98"/>
-      <c r="E1" s="98"/>
-      <c r="F1" s="98"/>
-      <c r="G1" s="98"/>
-      <c r="H1" s="98"/>
-      <c r="I1" s="99"/>
+      <c r="A1" s="95" t="s">
+        <v>72</v>
+      </c>
+      <c r="B1" s="96"/>
+      <c r="C1" s="96"/>
+      <c r="D1" s="96"/>
+      <c r="E1" s="96"/>
+      <c r="F1" s="96"/>
+      <c r="G1" s="96"/>
+      <c r="H1" s="96"/>
+      <c r="I1" s="97"/>
     </row>
     <row r="2" spans="1:13" s="2" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1" t="s">
@@ -1647,7 +1644,7 @@
       <c r="A3" s="100">
         <v>16</v>
       </c>
-      <c r="B3" s="101" t="s">
+      <c r="B3" s="103" t="s">
         <v>14</v>
       </c>
       <c r="C3" s="66">
@@ -1680,7 +1677,7 @@
     </row>
     <row r="4" spans="1:13" ht="81.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="93"/>
-      <c r="B4" s="109"/>
+      <c r="B4" s="104"/>
       <c r="C4" s="64" t="s">
         <v>11</v>
       </c>
@@ -1691,11 +1688,11 @@
         <v>11</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G4" s="8"/>
       <c r="H4" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I4" s="9"/>
     </row>
@@ -1703,7 +1700,7 @@
       <c r="A5" s="93">
         <v>15</v>
       </c>
-      <c r="B5" s="109"/>
+      <c r="B5" s="104"/>
       <c r="C5" s="10">
         <f>I3 + 1</f>
         <v>21</v>
@@ -1735,22 +1732,22 @@
     </row>
     <row r="6" spans="1:13" ht="82.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="93"/>
-      <c r="B6" s="109"/>
+      <c r="B6" s="104"/>
       <c r="C6" s="63" t="s">
         <v>10</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E6" s="8"/>
       <c r="F6" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="G6" s="61" t="s">
+        <v>68</v>
+      </c>
+      <c r="H6" s="7" t="s">
         <v>70</v>
-      </c>
-      <c r="G6" s="61" t="s">
-        <v>69</v>
-      </c>
-      <c r="H6" s="7" t="s">
-        <v>72</v>
       </c>
       <c r="I6" s="92"/>
     </row>
@@ -1758,7 +1755,7 @@
       <c r="A7" s="93">
         <v>14</v>
       </c>
-      <c r="B7" s="109"/>
+      <c r="B7" s="104"/>
       <c r="C7" s="10">
         <f>I5 + 1</f>
         <v>28</v>
@@ -1789,20 +1786,20 @@
     </row>
     <row r="8" spans="1:13" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="94"/>
-      <c r="B8" s="102"/>
+      <c r="B8" s="105"/>
       <c r="C8" s="90" t="s">
         <v>21</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E8" s="30"/>
       <c r="F8" s="55" t="s">
-        <v>29</v>
+        <v>71</v>
       </c>
       <c r="G8" s="17"/>
       <c r="H8" s="16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I8" s="62" t="s">
         <v>27</v>
@@ -1812,7 +1809,7 @@
       <c r="A9" s="100">
         <v>13</v>
       </c>
-      <c r="B9" s="110" t="s">
+      <c r="B9" s="106" t="s">
         <v>15</v>
       </c>
       <c r="C9" s="20">
@@ -1846,20 +1843,20 @@
     </row>
     <row r="10" spans="1:13" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="93"/>
-      <c r="B10" s="111"/>
+      <c r="B10" s="107"/>
       <c r="C10" s="63" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D10" s="18" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E10" s="17"/>
       <c r="F10" s="18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G10" s="17"/>
       <c r="H10" s="18" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I10" s="19"/>
     </row>
@@ -1867,7 +1864,7 @@
       <c r="A11" s="93">
         <v>12</v>
       </c>
-      <c r="B11" s="111"/>
+      <c r="B11" s="107"/>
       <c r="C11" s="24">
         <f>I9 + 1</f>
         <v>11</v>
@@ -1899,16 +1896,16 @@
     </row>
     <row r="12" spans="1:13" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="93"/>
-      <c r="B12" s="111"/>
+      <c r="B12" s="107"/>
       <c r="C12" s="63" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D12" s="18" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E12" s="17"/>
       <c r="F12" s="18" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G12" s="17"/>
       <c r="H12" s="18" t="s">
@@ -1920,7 +1917,7 @@
       <c r="A13" s="93">
         <v>11</v>
       </c>
-      <c r="B13" s="111"/>
+      <c r="B13" s="107"/>
       <c r="C13" s="24">
         <f>I11 + 1</f>
         <v>18</v>
@@ -1952,18 +1949,18 @@
     </row>
     <row r="14" spans="1:13" ht="83.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="93"/>
-      <c r="B14" s="111"/>
+      <c r="B14" s="107"/>
       <c r="C14" s="24"/>
       <c r="D14" s="18" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E14" s="17"/>
       <c r="F14" s="51" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G14" s="16"/>
       <c r="H14" s="18" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I14" s="62" t="s">
         <v>9</v>
@@ -1975,7 +1972,7 @@
       <c r="A15" s="93">
         <v>10</v>
       </c>
-      <c r="B15" s="111"/>
+      <c r="B15" s="107"/>
       <c r="C15" s="64">
         <f>I13 + 1</f>
         <v>25</v>
@@ -2006,9 +2003,9 @@
     </row>
     <row r="16" spans="1:13" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="94"/>
-      <c r="B16" s="112"/>
+      <c r="B16" s="108"/>
       <c r="C16" s="71" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D16" s="72" t="str">
         <f t="shared" ref="D16:I16" si="2">C16</f>
@@ -2051,7 +2048,7 @@
       <c r="B18" s="35"/>
       <c r="D18" s="38"/>
       <c r="E18" s="91" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F18" s="38"/>
       <c r="G18" s="38"/>
@@ -2063,7 +2060,7 @@
       <c r="B19" s="40"/>
       <c r="D19" s="34"/>
       <c r="E19" s="82" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F19" s="34"/>
       <c r="G19" s="34"/>
@@ -2075,7 +2072,7 @@
       <c r="B20" s="35"/>
       <c r="D20" s="38"/>
       <c r="E20" s="83" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F20" s="38"/>
       <c r="G20" s="38"/>
@@ -2087,7 +2084,7 @@
       <c r="B21" s="35"/>
       <c r="D21" s="38"/>
       <c r="E21" s="84" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F21" s="38"/>
       <c r="G21" s="38"/>
@@ -2099,7 +2096,7 @@
       <c r="B22" s="35"/>
       <c r="D22" s="38"/>
       <c r="E22" s="85" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F22" s="38"/>
       <c r="G22" s="38"/>
@@ -2112,7 +2109,7 @@
       <c r="C23" s="80"/>
       <c r="D23" s="38"/>
       <c r="E23" s="86" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F23" s="38"/>
       <c r="G23" s="38"/>
@@ -2153,19 +2150,19 @@
       <c r="I26" s="38"/>
     </row>
     <row r="27" spans="1:11" s="36" customFormat="1" ht="57.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="97" t="str">
+      <c r="A27" s="95" t="str">
         <f>A1</f>
         <v>CS320: SW Engineering - Spring 2018 Schedule
-(as of 1-26-2018, subject to change)</v>
-      </c>
-      <c r="B27" s="98"/>
-      <c r="C27" s="98"/>
-      <c r="D27" s="98"/>
-      <c r="E27" s="98"/>
-      <c r="F27" s="98"/>
-      <c r="G27" s="98"/>
-      <c r="H27" s="98"/>
-      <c r="I27" s="99"/>
+(as of 1-29-2018, subject to change)</v>
+      </c>
+      <c r="B27" s="96"/>
+      <c r="C27" s="96"/>
+      <c r="D27" s="96"/>
+      <c r="E27" s="96"/>
+      <c r="F27" s="96"/>
+      <c r="G27" s="96"/>
+      <c r="H27" s="96"/>
+      <c r="I27" s="97"/>
     </row>
     <row r="28" spans="1:11" s="2" customFormat="1" ht="17.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="str">
@@ -2206,11 +2203,11 @@
       </c>
     </row>
     <row r="29" spans="1:11" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="106">
+      <c r="A29" s="98">
         <v>10</v>
       </c>
-      <c r="B29" s="107" t="s">
-        <v>45</v>
+      <c r="B29" s="101" t="s">
+        <v>44</v>
       </c>
       <c r="C29" s="64">
         <f>C15</f>
@@ -2241,10 +2238,10 @@
       </c>
     </row>
     <row r="30" spans="1:11" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="96"/>
-      <c r="B30" s="108"/>
+      <c r="A30" s="99"/>
+      <c r="B30" s="102"/>
       <c r="C30" s="77" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D30" s="75" t="str">
         <f t="shared" ref="D30" si="5">C30</f>
@@ -2275,7 +2272,7 @@
       <c r="A31" s="100">
         <v>9</v>
       </c>
-      <c r="B31" s="101" t="s">
+      <c r="B31" s="103" t="s">
         <v>16</v>
       </c>
       <c r="C31" s="64">
@@ -2309,23 +2306,23 @@
     </row>
     <row r="32" spans="1:11" ht="86.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="93"/>
-      <c r="B32" s="109"/>
+      <c r="B32" s="104"/>
       <c r="C32" s="64" t="str">
         <f>I30</f>
         <v>WINTER BREAK</v>
       </c>
       <c r="D32" s="27" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E32" s="61" t="s">
         <v>25</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G32" s="7"/>
       <c r="H32" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I32" s="61" t="s">
         <v>24</v>
@@ -2336,7 +2333,7 @@
       <c r="A33" s="93">
         <v>8</v>
       </c>
-      <c r="B33" s="109"/>
+      <c r="B33" s="104"/>
       <c r="C33" s="28">
         <f>I31 + 1</f>
         <v>11</v>
@@ -2368,18 +2365,18 @@
     </row>
     <row r="34" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="93"/>
-      <c r="B34" s="109"/>
+      <c r="B34" s="104"/>
       <c r="C34" s="10"/>
       <c r="D34" s="45" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E34" s="7"/>
       <c r="F34" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G34" s="7"/>
       <c r="H34" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I34" s="62" t="s">
         <v>26</v>
@@ -2390,7 +2387,7 @@
       <c r="A35" s="93">
         <v>7</v>
       </c>
-      <c r="B35" s="109"/>
+      <c r="B35" s="104"/>
       <c r="C35" s="10">
         <f>I33 + 1</f>
         <v>18</v>
@@ -2422,14 +2419,14 @@
     </row>
     <row r="36" spans="1:11" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="93"/>
-      <c r="B36" s="109"/>
+      <c r="B36" s="104"/>
       <c r="C36" s="10"/>
       <c r="D36" s="32" t="s">
         <v>19</v>
       </c>
       <c r="E36" s="8"/>
       <c r="F36" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G36" s="7"/>
       <c r="H36" s="7" t="s">
@@ -2441,7 +2438,7 @@
       <c r="A37" s="93">
         <v>6</v>
       </c>
-      <c r="B37" s="109"/>
+      <c r="B37" s="104"/>
       <c r="C37" s="10">
         <f>I35 + 1</f>
         <v>25</v>
@@ -2473,10 +2470,10 @@
     </row>
     <row r="38" spans="1:11" ht="44.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="94"/>
-      <c r="B38" s="102"/>
+      <c r="B38" s="105"/>
       <c r="C38" s="29"/>
       <c r="D38" s="44" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E38" s="30"/>
       <c r="F38" s="56" t="s">
@@ -2496,7 +2493,7 @@
       <c r="A39" s="100">
         <v>5</v>
       </c>
-      <c r="B39" s="103" t="s">
+      <c r="B39" s="110" t="s">
         <v>17</v>
       </c>
       <c r="C39" s="64">
@@ -2529,7 +2526,7 @@
     </row>
     <row r="40" spans="1:11" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="93"/>
-      <c r="B40" s="104"/>
+      <c r="B40" s="111"/>
       <c r="C40" s="64" t="s">
         <v>7</v>
       </c>
@@ -2542,17 +2539,17 @@
       </c>
       <c r="G40" s="17"/>
       <c r="H40" s="88" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I40" s="62" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="41" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="93">
         <v>4</v>
       </c>
-      <c r="B41" s="104"/>
+      <c r="B41" s="111"/>
       <c r="C41" s="24">
         <f>I39 + 1</f>
         <v>8</v>
@@ -2584,10 +2581,10 @@
     </row>
     <row r="42" spans="1:11" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="93"/>
-      <c r="B42" s="104"/>
+      <c r="B42" s="111"/>
       <c r="C42" s="87"/>
       <c r="D42" s="45" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E42" s="17"/>
       <c r="F42" s="31" t="s">
@@ -2603,7 +2600,7 @@
       <c r="A43" s="93">
         <v>3</v>
       </c>
-      <c r="B43" s="104"/>
+      <c r="B43" s="111"/>
       <c r="C43" s="59">
         <f>I41 + 1</f>
         <v>15</v>
@@ -2635,10 +2632,10 @@
     </row>
     <row r="44" spans="1:11" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="93"/>
-      <c r="B44" s="104"/>
+      <c r="B44" s="111"/>
       <c r="C44" s="57"/>
       <c r="D44" s="32" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E44" s="17"/>
       <c r="F44" s="31" t="s">
@@ -2654,7 +2651,7 @@
       <c r="A45" s="93">
         <v>2</v>
       </c>
-      <c r="B45" s="104"/>
+      <c r="B45" s="111"/>
       <c r="C45" s="24">
         <f>I43 + 1</f>
         <v>22</v>
@@ -2686,13 +2683,13 @@
     </row>
     <row r="46" spans="1:11" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="93"/>
-      <c r="B46" s="104"/>
+      <c r="B46" s="111"/>
       <c r="C46" s="23"/>
       <c r="D46" s="45" t="s">
+        <v>64</v>
+      </c>
+      <c r="E46" s="61" t="s">
         <v>65</v>
-      </c>
-      <c r="E46" s="61" t="s">
-        <v>66</v>
       </c>
       <c r="F46" s="31" t="s">
         <v>8</v>
@@ -2708,7 +2705,7 @@
         <f>A50 + 1</f>
         <v>1</v>
       </c>
-      <c r="B47" s="104"/>
+      <c r="B47" s="111"/>
       <c r="C47" s="24">
         <f>I45 + 1</f>
         <v>29</v>
@@ -2739,7 +2736,7 @@
     </row>
     <row r="48" spans="1:11" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="94"/>
-      <c r="B48" s="105"/>
+      <c r="B48" s="112"/>
       <c r="C48" s="48"/>
       <c r="D48" s="58" t="s">
         <v>8</v>
@@ -2755,10 +2752,10 @@
       </c>
     </row>
     <row r="49" spans="1:9" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="95">
+      <c r="A49" s="109">
         <v>0</v>
       </c>
-      <c r="B49" s="101" t="s">
+      <c r="B49" s="103" t="s">
         <v>5</v>
       </c>
       <c r="C49" s="10">
@@ -2791,12 +2788,12 @@
       </c>
     </row>
     <row r="50" spans="1:9" ht="129.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="96"/>
-      <c r="B50" s="102"/>
+      <c r="A50" s="99"/>
+      <c r="B50" s="105"/>
       <c r="C50" s="14"/>
       <c r="D50" s="14"/>
       <c r="E50" s="89" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F50" s="33" t="s">
         <v>28</v>
@@ -2808,6 +2805,18 @@
     <row r="51" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="A47:A48"/>
+    <mergeCell ref="A49:A50"/>
+    <mergeCell ref="A27:I27"/>
+    <mergeCell ref="A33:A34"/>
+    <mergeCell ref="A35:A36"/>
+    <mergeCell ref="A37:A38"/>
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="A41:A42"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="B39:B48"/>
     <mergeCell ref="A13:A14"/>
     <mergeCell ref="A15:A16"/>
     <mergeCell ref="A1:I1"/>
@@ -2822,18 +2831,6 @@
     <mergeCell ref="B31:B38"/>
     <mergeCell ref="B3:B8"/>
     <mergeCell ref="B9:B16"/>
-    <mergeCell ref="A43:A44"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="A47:A48"/>
-    <mergeCell ref="A49:A50"/>
-    <mergeCell ref="A27:I27"/>
-    <mergeCell ref="A33:A34"/>
-    <mergeCell ref="A35:A36"/>
-    <mergeCell ref="A37:A38"/>
-    <mergeCell ref="A39:A40"/>
-    <mergeCell ref="A41:A42"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="B39:B48"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="5" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
moed due date for Lab04
</commit_message>
<xml_diff>
--- a/CS320-Spring2018Calendar.xlsx
+++ b/CS320-Spring2018Calendar.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="74">
   <si>
     <t>Monday</t>
   </si>
@@ -342,10 +342,6 @@
 (Scrum Guide)</t>
   </si>
   <si>
-    <t>CS320: SW Engineering - Spring 2018 Schedule
-(as of 2-4-2018, subject to change)</t>
-  </si>
-  <si>
     <t>Lecture 8: Requirements, Use Cases
 (UD: Chapter 9)
 Use Case Exercise
@@ -373,6 +369,15 @@
     <t>Team Session:
 Use Cases
 (in class)</t>
+  </si>
+  <si>
+    <t>CS320: SW Engineering - Spring 2018 Schedule
+(as of 3-6-2018, subject to change)</t>
+  </si>
+  <si>
+    <t>AndCulture.com
+Presentation
+(Guest Lecturers)</t>
   </si>
 </sst>
 </file>
@@ -1228,6 +1233,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1237,13 +1248,25 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1252,15 +1275,9 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
@@ -1268,18 +1285,6 @@
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1588,8 +1593,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G42" sqref="G42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1607,17 +1612,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="57.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="95" t="s">
-        <v>66</v>
-      </c>
-      <c r="B1" s="96"/>
-      <c r="C1" s="96"/>
-      <c r="D1" s="96"/>
-      <c r="E1" s="96"/>
-      <c r="F1" s="96"/>
-      <c r="G1" s="96"/>
-      <c r="H1" s="96"/>
-      <c r="I1" s="97"/>
+      <c r="A1" s="97" t="s">
+        <v>72</v>
+      </c>
+      <c r="B1" s="98"/>
+      <c r="C1" s="98"/>
+      <c r="D1" s="98"/>
+      <c r="E1" s="98"/>
+      <c r="F1" s="98"/>
+      <c r="G1" s="98"/>
+      <c r="H1" s="98"/>
+      <c r="I1" s="99"/>
     </row>
     <row r="2" spans="1:13" s="2" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -1650,7 +1655,7 @@
       <c r="A3" s="100">
         <v>16</v>
       </c>
-      <c r="B3" s="103" t="s">
+      <c r="B3" s="101" t="s">
         <v>13</v>
       </c>
       <c r="C3" s="66">
@@ -1683,7 +1688,7 @@
     </row>
     <row r="4" spans="1:13" ht="81.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="93"/>
-      <c r="B4" s="104"/>
+      <c r="B4" s="109"/>
       <c r="C4" s="64" t="s">
         <v>10</v>
       </c>
@@ -1706,7 +1711,7 @@
       <c r="A5" s="93">
         <v>15</v>
       </c>
-      <c r="B5" s="104"/>
+      <c r="B5" s="109"/>
       <c r="C5" s="10">
         <f>I3 + 1</f>
         <v>21</v>
@@ -1738,7 +1743,7 @@
     </row>
     <row r="6" spans="1:13" ht="82.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="93"/>
-      <c r="B6" s="104"/>
+      <c r="B6" s="109"/>
       <c r="C6" s="63" t="s">
         <v>9</v>
       </c>
@@ -1761,7 +1766,7 @@
       <c r="A7" s="93">
         <v>14</v>
       </c>
-      <c r="B7" s="104"/>
+      <c r="B7" s="109"/>
       <c r="C7" s="10">
         <f>I5 + 1</f>
         <v>28</v>
@@ -1792,7 +1797,7 @@
     </row>
     <row r="8" spans="1:13" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="94"/>
-      <c r="B8" s="105"/>
+      <c r="B8" s="102"/>
       <c r="C8" s="90" t="s">
         <v>20</v>
       </c>
@@ -1805,7 +1810,7 @@
       </c>
       <c r="G8" s="17"/>
       <c r="H8" s="16" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I8" s="62" t="s">
         <v>26</v>
@@ -1815,7 +1820,7 @@
       <c r="A9" s="100">
         <v>13</v>
       </c>
-      <c r="B9" s="106" t="s">
+      <c r="B9" s="110" t="s">
         <v>14</v>
       </c>
       <c r="C9" s="20">
@@ -1849,16 +1854,16 @@
     </row>
     <row r="10" spans="1:13" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="93"/>
-      <c r="B10" s="107"/>
+      <c r="B10" s="111"/>
       <c r="C10" s="63" t="s">
         <v>61</v>
       </c>
       <c r="D10" s="18" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E10" s="17"/>
       <c r="F10" s="18" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G10" s="17"/>
       <c r="H10" s="18" t="s">
@@ -1870,7 +1875,7 @@
       <c r="A11" s="93">
         <v>12</v>
       </c>
-      <c r="B11" s="107"/>
+      <c r="B11" s="111"/>
       <c r="C11" s="24">
         <f>I9 + 1</f>
         <v>11</v>
@@ -1902,20 +1907,20 @@
     </row>
     <row r="12" spans="1:13" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="93"/>
-      <c r="B12" s="107"/>
+      <c r="B12" s="111"/>
       <c r="C12" s="63" t="s">
         <v>54</v>
       </c>
       <c r="D12" s="18" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E12" s="17"/>
       <c r="F12" s="18" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G12" s="17"/>
       <c r="H12" s="18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I12" s="19"/>
     </row>
@@ -1923,7 +1928,7 @@
       <c r="A13" s="93">
         <v>11</v>
       </c>
-      <c r="B13" s="107"/>
+      <c r="B13" s="111"/>
       <c r="C13" s="24">
         <f>I11 + 1</f>
         <v>18</v>
@@ -1955,7 +1960,7 @@
     </row>
     <row r="14" spans="1:13" ht="83.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="93"/>
-      <c r="B14" s="107"/>
+      <c r="B14" s="111"/>
       <c r="C14" s="24"/>
       <c r="D14" s="18" t="s">
         <v>28</v>
@@ -1978,7 +1983,7 @@
       <c r="A15" s="93">
         <v>10</v>
       </c>
-      <c r="B15" s="107"/>
+      <c r="B15" s="111"/>
       <c r="C15" s="64">
         <f>I13 + 1</f>
         <v>25</v>
@@ -2009,7 +2014,7 @@
     </row>
     <row r="16" spans="1:13" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="94"/>
-      <c r="B16" s="108"/>
+      <c r="B16" s="112"/>
       <c r="C16" s="71" t="s">
         <v>41</v>
       </c>
@@ -2156,19 +2161,19 @@
       <c r="I26" s="38"/>
     </row>
     <row r="27" spans="1:11" s="36" customFormat="1" ht="57.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="95" t="str">
+      <c r="A27" s="97" t="str">
         <f>A1</f>
         <v>CS320: SW Engineering - Spring 2018 Schedule
-(as of 2-4-2018, subject to change)</v>
-      </c>
-      <c r="B27" s="96"/>
-      <c r="C27" s="96"/>
-      <c r="D27" s="96"/>
-      <c r="E27" s="96"/>
-      <c r="F27" s="96"/>
-      <c r="G27" s="96"/>
-      <c r="H27" s="96"/>
-      <c r="I27" s="97"/>
+(as of 3-6-2018, subject to change)</v>
+      </c>
+      <c r="B27" s="98"/>
+      <c r="C27" s="98"/>
+      <c r="D27" s="98"/>
+      <c r="E27" s="98"/>
+      <c r="F27" s="98"/>
+      <c r="G27" s="98"/>
+      <c r="H27" s="98"/>
+      <c r="I27" s="99"/>
     </row>
     <row r="28" spans="1:11" s="2" customFormat="1" ht="17.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="str">
@@ -2209,10 +2214,10 @@
       </c>
     </row>
     <row r="29" spans="1:11" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="98">
+      <c r="A29" s="106">
         <v>10</v>
       </c>
-      <c r="B29" s="101" t="s">
+      <c r="B29" s="107" t="s">
         <v>43</v>
       </c>
       <c r="C29" s="64">
@@ -2244,8 +2249,8 @@
       </c>
     </row>
     <row r="30" spans="1:11" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="99"/>
-      <c r="B30" s="102"/>
+      <c r="A30" s="96"/>
+      <c r="B30" s="108"/>
       <c r="C30" s="77" t="s">
         <v>41</v>
       </c>
@@ -2278,7 +2283,7 @@
       <c r="A31" s="100">
         <v>9</v>
       </c>
-      <c r="B31" s="103" t="s">
+      <c r="B31" s="101" t="s">
         <v>15</v>
       </c>
       <c r="C31" s="64">
@@ -2312,7 +2317,7 @@
     </row>
     <row r="32" spans="1:11" ht="86.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="93"/>
-      <c r="B32" s="104"/>
+      <c r="B32" s="109"/>
       <c r="C32" s="64" t="str">
         <f>I30</f>
         <v>WINTER BREAK</v>
@@ -2320,13 +2325,13 @@
       <c r="D32" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="E32" s="61" t="s">
-        <v>24</v>
-      </c>
+      <c r="E32" s="7"/>
       <c r="F32" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="G32" s="7"/>
+      <c r="G32" s="61" t="s">
+        <v>24</v>
+      </c>
       <c r="H32" s="7" t="s">
         <v>39</v>
       </c>
@@ -2339,7 +2344,7 @@
       <c r="A33" s="93">
         <v>8</v>
       </c>
-      <c r="B33" s="104"/>
+      <c r="B33" s="109"/>
       <c r="C33" s="28">
         <f>I31 + 1</f>
         <v>11</v>
@@ -2371,7 +2376,7 @@
     </row>
     <row r="34" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="93"/>
-      <c r="B34" s="104"/>
+      <c r="B34" s="109"/>
       <c r="C34" s="10"/>
       <c r="D34" s="45" t="s">
         <v>55</v>
@@ -2393,7 +2398,7 @@
       <c r="A35" s="93">
         <v>7</v>
       </c>
-      <c r="B35" s="104"/>
+      <c r="B35" s="109"/>
       <c r="C35" s="10">
         <f>I33 + 1</f>
         <v>18</v>
@@ -2425,7 +2430,7 @@
     </row>
     <row r="36" spans="1:11" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="93"/>
-      <c r="B36" s="104"/>
+      <c r="B36" s="109"/>
       <c r="C36" s="10"/>
       <c r="D36" s="32" t="s">
         <v>18</v>
@@ -2444,7 +2449,7 @@
       <c r="A37" s="93">
         <v>6</v>
       </c>
-      <c r="B37" s="104"/>
+      <c r="B37" s="109"/>
       <c r="C37" s="10">
         <f>I35 + 1</f>
         <v>25</v>
@@ -2476,7 +2481,7 @@
     </row>
     <row r="38" spans="1:11" ht="44.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="94"/>
-      <c r="B38" s="105"/>
+      <c r="B38" s="102"/>
       <c r="C38" s="29"/>
       <c r="D38" s="44" t="s">
         <v>56</v>
@@ -2499,7 +2504,7 @@
       <c r="A39" s="100">
         <v>5</v>
       </c>
-      <c r="B39" s="110" t="s">
+      <c r="B39" s="103" t="s">
         <v>16</v>
       </c>
       <c r="C39" s="64">
@@ -2532,7 +2537,7 @@
     </row>
     <row r="40" spans="1:11" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="93"/>
-      <c r="B40" s="111"/>
+      <c r="B40" s="104"/>
       <c r="C40" s="64" t="s">
         <v>6</v>
       </c>
@@ -2555,7 +2560,7 @@
       <c r="A41" s="93">
         <v>4</v>
       </c>
-      <c r="B41" s="111"/>
+      <c r="B41" s="104"/>
       <c r="C41" s="24">
         <f>I39 + 1</f>
         <v>8</v>
@@ -2587,14 +2592,14 @@
     </row>
     <row r="42" spans="1:11" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="93"/>
-      <c r="B42" s="111"/>
+      <c r="B42" s="104"/>
       <c r="C42" s="87"/>
       <c r="D42" s="45" t="s">
         <v>57</v>
       </c>
       <c r="E42" s="17"/>
       <c r="F42" s="31" t="s">
-        <v>7</v>
+        <v>73</v>
       </c>
       <c r="G42" s="53"/>
       <c r="H42" s="31" t="s">
@@ -2606,7 +2611,7 @@
       <c r="A43" s="93">
         <v>3</v>
       </c>
-      <c r="B43" s="111"/>
+      <c r="B43" s="104"/>
       <c r="C43" s="59">
         <f>I41 + 1</f>
         <v>15</v>
@@ -2638,7 +2643,7 @@
     </row>
     <row r="44" spans="1:11" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="93"/>
-      <c r="B44" s="111"/>
+      <c r="B44" s="104"/>
       <c r="C44" s="57"/>
       <c r="D44" s="32" t="s">
         <v>53</v>
@@ -2657,7 +2662,7 @@
       <c r="A45" s="93">
         <v>2</v>
       </c>
-      <c r="B45" s="111"/>
+      <c r="B45" s="104"/>
       <c r="C45" s="24">
         <f>I43 + 1</f>
         <v>22</v>
@@ -2689,7 +2694,7 @@
     </row>
     <row r="46" spans="1:11" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="93"/>
-      <c r="B46" s="111"/>
+      <c r="B46" s="104"/>
       <c r="C46" s="23"/>
       <c r="D46" s="45" t="s">
         <v>58</v>
@@ -2711,7 +2716,7 @@
         <f>A50 + 1</f>
         <v>1</v>
       </c>
-      <c r="B47" s="111"/>
+      <c r="B47" s="104"/>
       <c r="C47" s="24">
         <f>I45 + 1</f>
         <v>29</v>
@@ -2742,7 +2747,7 @@
     </row>
     <row r="48" spans="1:11" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="94"/>
-      <c r="B48" s="112"/>
+      <c r="B48" s="105"/>
       <c r="C48" s="48"/>
       <c r="D48" s="58" t="s">
         <v>7</v>
@@ -2758,10 +2763,10 @@
       </c>
     </row>
     <row r="49" spans="1:9" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="109">
+      <c r="A49" s="95">
         <v>0</v>
       </c>
-      <c r="B49" s="103" t="s">
+      <c r="B49" s="101" t="s">
         <v>5</v>
       </c>
       <c r="C49" s="10">
@@ -2794,8 +2799,8 @@
       </c>
     </row>
     <row r="50" spans="1:9" ht="129.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="99"/>
-      <c r="B50" s="105"/>
+      <c r="A50" s="96"/>
+      <c r="B50" s="102"/>
       <c r="C50" s="14"/>
       <c r="D50" s="14"/>
       <c r="E50" s="89" t="s">
@@ -2811,18 +2816,6 @@
     <row r="51" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="A43:A44"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="A47:A48"/>
-    <mergeCell ref="A49:A50"/>
-    <mergeCell ref="A27:I27"/>
-    <mergeCell ref="A33:A34"/>
-    <mergeCell ref="A35:A36"/>
-    <mergeCell ref="A37:A38"/>
-    <mergeCell ref="A39:A40"/>
-    <mergeCell ref="A41:A42"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="B39:B48"/>
     <mergeCell ref="A13:A14"/>
     <mergeCell ref="A15:A16"/>
     <mergeCell ref="A1:I1"/>
@@ -2837,6 +2830,18 @@
     <mergeCell ref="B31:B38"/>
     <mergeCell ref="B3:B8"/>
     <mergeCell ref="B9:B16"/>
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="A47:A48"/>
+    <mergeCell ref="A49:A50"/>
+    <mergeCell ref="A27:I27"/>
+    <mergeCell ref="A33:A34"/>
+    <mergeCell ref="A35:A36"/>
+    <mergeCell ref="A37:A38"/>
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="A41:A42"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="B39:B48"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="5" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
updated schedules due to snow day
</commit_message>
<xml_diff>
--- a/CS320-Spring2018Calendar.xlsx
+++ b/CS320-Spring2018Calendar.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="75">
   <si>
     <t>Monday</t>
   </si>
@@ -378,6 +378,10 @@
     <t>AndCulture.com
 Presentation
 (Guest Lecturers)</t>
+  </si>
+  <si>
+    <t>WOO HOO
+A SNOW DAY…!</t>
   </si>
 </sst>
 </file>
@@ -949,7 +953,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="113">
+  <cellXfs count="112">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1080,9 +1084,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1233,30 +1234,51 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
@@ -1264,27 +1286,6 @@
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1593,8 +1594,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G42" sqref="G42"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F42" sqref="F42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1612,17 +1613,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="57.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="97" t="s">
+      <c r="A1" s="94" t="s">
         <v>72</v>
       </c>
-      <c r="B1" s="98"/>
-      <c r="C1" s="98"/>
-      <c r="D1" s="98"/>
-      <c r="E1" s="98"/>
-      <c r="F1" s="98"/>
-      <c r="G1" s="98"/>
-      <c r="H1" s="98"/>
-      <c r="I1" s="99"/>
+      <c r="B1" s="95"/>
+      <c r="C1" s="95"/>
+      <c r="D1" s="95"/>
+      <c r="E1" s="95"/>
+      <c r="F1" s="95"/>
+      <c r="G1" s="95"/>
+      <c r="H1" s="95"/>
+      <c r="I1" s="96"/>
     </row>
     <row r="2" spans="1:13" s="2" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -1652,20 +1653,20 @@
       </c>
     </row>
     <row r="3" spans="1:13" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="100">
+      <c r="A3" s="99">
         <v>16</v>
       </c>
-      <c r="B3" s="101" t="s">
+      <c r="B3" s="102" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="66">
+      <c r="C3" s="65">
         <v>14</v>
       </c>
-      <c r="D3" s="67">
+      <c r="D3" s="66">
         <f>C3 + 1</f>
         <v>15</v>
       </c>
-      <c r="E3" s="67">
+      <c r="E3" s="66">
         <f t="shared" ref="E3:I3" si="0">D3 + 1</f>
         <v>16</v>
       </c>
@@ -1687,15 +1688,15 @@
       </c>
     </row>
     <row r="4" spans="1:13" ht="81.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="93"/>
-      <c r="B4" s="109"/>
-      <c r="C4" s="64" t="s">
+      <c r="A4" s="92"/>
+      <c r="B4" s="103"/>
+      <c r="C4" s="63" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="65" t="s">
+      <c r="D4" s="64" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="65" t="s">
+      <c r="E4" s="64" t="s">
         <v>10</v>
       </c>
       <c r="F4" s="7" t="s">
@@ -1708,10 +1709,10 @@
       <c r="I4" s="9"/>
     </row>
     <row r="5" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="93">
+      <c r="A5" s="92">
         <v>15</v>
       </c>
-      <c r="B5" s="109"/>
+      <c r="B5" s="103"/>
       <c r="C5" s="10">
         <f>I3 + 1</f>
         <v>21</v>
@@ -1742,9 +1743,9 @@
       </c>
     </row>
     <row r="6" spans="1:13" ht="82.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="93"/>
-      <c r="B6" s="109"/>
-      <c r="C6" s="63" t="s">
+      <c r="A6" s="92"/>
+      <c r="B6" s="103"/>
+      <c r="C6" s="62" t="s">
         <v>9</v>
       </c>
       <c r="D6" s="7" t="s">
@@ -1754,19 +1755,19 @@
       <c r="F6" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="G6" s="61" t="s">
+      <c r="G6" s="60" t="s">
         <v>62</v>
       </c>
       <c r="H6" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="I6" s="92"/>
+      <c r="I6" s="91"/>
     </row>
     <row r="7" spans="1:13" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="93">
+      <c r="A7" s="92">
         <v>14</v>
       </c>
-      <c r="B7" s="109"/>
+      <c r="B7" s="103"/>
       <c r="C7" s="10">
         <f>I5 + 1</f>
         <v>28</v>
@@ -1779,7 +1780,7 @@
         <f t="shared" si="1"/>
         <v>30</v>
       </c>
-      <c r="F7" s="52">
+      <c r="F7" s="51">
         <f>E7+1</f>
         <v>31</v>
       </c>
@@ -1796,31 +1797,31 @@
       </c>
     </row>
     <row r="8" spans="1:13" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="94"/>
-      <c r="B8" s="102"/>
-      <c r="C8" s="90" t="s">
+      <c r="A8" s="93"/>
+      <c r="B8" s="104"/>
+      <c r="C8" s="89" t="s">
         <v>20</v>
       </c>
       <c r="D8" s="14" t="s">
         <v>47</v>
       </c>
       <c r="E8" s="30"/>
-      <c r="F8" s="55" t="s">
+      <c r="F8" s="54" t="s">
         <v>65</v>
       </c>
       <c r="G8" s="17"/>
       <c r="H8" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="I8" s="62" t="s">
+      <c r="I8" s="61" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="100">
+      <c r="A9" s="99">
         <v>13</v>
       </c>
-      <c r="B9" s="110" t="s">
+      <c r="B9" s="105" t="s">
         <v>14</v>
       </c>
       <c r="C9" s="20">
@@ -1853,9 +1854,9 @@
       </c>
     </row>
     <row r="10" spans="1:13" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="93"/>
-      <c r="B10" s="111"/>
-      <c r="C10" s="63" t="s">
+      <c r="A10" s="92"/>
+      <c r="B10" s="106"/>
+      <c r="C10" s="62" t="s">
         <v>61</v>
       </c>
       <c r="D10" s="18" t="s">
@@ -1872,10 +1873,10 @@
       <c r="I10" s="19"/>
     </row>
     <row r="11" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="93">
+      <c r="A11" s="92">
         <v>12</v>
       </c>
-      <c r="B11" s="111"/>
+      <c r="B11" s="106"/>
       <c r="C11" s="24">
         <f>I9 + 1</f>
         <v>11</v>
@@ -1906,9 +1907,9 @@
       </c>
     </row>
     <row r="12" spans="1:13" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="93"/>
-      <c r="B12" s="111"/>
-      <c r="C12" s="63" t="s">
+      <c r="A12" s="92"/>
+      <c r="B12" s="106"/>
+      <c r="C12" s="62" t="s">
         <v>54</v>
       </c>
       <c r="D12" s="18" t="s">
@@ -1925,10 +1926,10 @@
       <c r="I12" s="19"/>
     </row>
     <row r="13" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="93">
+      <c r="A13" s="92">
         <v>11</v>
       </c>
-      <c r="B13" s="111"/>
+      <c r="B13" s="106"/>
       <c r="C13" s="24">
         <f>I11 + 1</f>
         <v>18</v>
@@ -1953,98 +1954,98 @@
         <f t="shared" si="1"/>
         <v>23</v>
       </c>
-      <c r="I13" s="69">
+      <c r="I13" s="68">
         <f t="shared" si="1"/>
         <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="83.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="93"/>
-      <c r="B14" s="111"/>
+      <c r="A14" s="92"/>
+      <c r="B14" s="106"/>
       <c r="C14" s="24"/>
       <c r="D14" s="18" t="s">
         <v>28</v>
       </c>
       <c r="E14" s="17"/>
-      <c r="F14" s="51" t="s">
+      <c r="F14" s="50" t="s">
         <v>29</v>
       </c>
       <c r="G14" s="16"/>
       <c r="H14" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="I14" s="62" t="s">
+      <c r="I14" s="61" t="s">
         <v>8</v>
       </c>
       <c r="L14" s="42"/>
       <c r="M14" s="42"/>
     </row>
     <row r="15" spans="1:13" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="93">
+      <c r="A15" s="92">
         <v>10</v>
       </c>
-      <c r="B15" s="111"/>
-      <c r="C15" s="64">
+      <c r="B15" s="106"/>
+      <c r="C15" s="63">
         <f>I13 + 1</f>
         <v>25</v>
       </c>
-      <c r="D15" s="65">
+      <c r="D15" s="64">
         <f>C15 + 1</f>
         <v>26</v>
       </c>
-      <c r="E15" s="68">
+      <c r="E15" s="67">
         <f t="shared" si="1"/>
         <v>27</v>
       </c>
-      <c r="F15" s="69">
+      <c r="F15" s="68">
         <f>E15 + 1</f>
         <v>28</v>
       </c>
-      <c r="G15" s="66">
+      <c r="G15" s="65">
         <v>1</v>
       </c>
-      <c r="H15" s="67">
+      <c r="H15" s="66">
         <f>G15 + 1</f>
         <v>2</v>
       </c>
-      <c r="I15" s="70">
+      <c r="I15" s="69">
         <f>H15 + 1</f>
         <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="94"/>
-      <c r="B16" s="112"/>
-      <c r="C16" s="71" t="s">
+      <c r="A16" s="93"/>
+      <c r="B16" s="107"/>
+      <c r="C16" s="70" t="s">
         <v>41</v>
       </c>
-      <c r="D16" s="72" t="str">
+      <c r="D16" s="71" t="str">
         <f t="shared" ref="D16:I16" si="2">C16</f>
         <v>WINTER BREAK</v>
       </c>
-      <c r="E16" s="73" t="str">
+      <c r="E16" s="72" t="str">
         <f t="shared" si="2"/>
         <v>WINTER BREAK</v>
       </c>
-      <c r="F16" s="74" t="str">
+      <c r="F16" s="73" t="str">
         <f>E16</f>
         <v>WINTER BREAK</v>
       </c>
-      <c r="G16" s="71" t="str">
+      <c r="G16" s="70" t="str">
         <f>F16</f>
         <v>WINTER BREAK</v>
       </c>
-      <c r="H16" s="75" t="str">
+      <c r="H16" s="74" t="str">
         <f>G16</f>
         <v>WINTER BREAK</v>
       </c>
-      <c r="I16" s="74" t="str">
+      <c r="I16" s="73" t="str">
         <f t="shared" si="2"/>
         <v>WINTER BREAK</v>
       </c>
     </row>
     <row r="17" spans="1:11" s="39" customFormat="1" ht="21.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="81"/>
+      <c r="A17" s="80"/>
       <c r="B17" s="35"/>
       <c r="C17" s="38"/>
       <c r="D17" s="38"/>
@@ -2055,10 +2056,10 @@
       <c r="I17" s="38"/>
     </row>
     <row r="18" spans="1:11" s="39" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="81"/>
+      <c r="A18" s="80"/>
       <c r="B18" s="35"/>
       <c r="D18" s="38"/>
-      <c r="E18" s="91" t="s">
+      <c r="E18" s="90" t="s">
         <v>50</v>
       </c>
       <c r="F18" s="38"/>
@@ -2067,10 +2068,10 @@
       <c r="I18" s="38"/>
     </row>
     <row r="19" spans="1:11" s="37" customFormat="1" ht="22.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="81"/>
+      <c r="A19" s="80"/>
       <c r="B19" s="40"/>
       <c r="D19" s="34"/>
-      <c r="E19" s="82" t="s">
+      <c r="E19" s="81" t="s">
         <v>42</v>
       </c>
       <c r="F19" s="34"/>
@@ -2079,10 +2080,10 @@
       <c r="I19" s="34"/>
     </row>
     <row r="20" spans="1:11" s="39" customFormat="1" ht="29.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="81"/>
+      <c r="A20" s="80"/>
       <c r="B20" s="35"/>
       <c r="D20" s="38"/>
-      <c r="E20" s="83" t="s">
+      <c r="E20" s="82" t="s">
         <v>44</v>
       </c>
       <c r="F20" s="38"/>
@@ -2091,10 +2092,10 @@
       <c r="I20" s="38"/>
     </row>
     <row r="21" spans="1:11" s="39" customFormat="1" ht="39" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="81"/>
+      <c r="A21" s="80"/>
       <c r="B21" s="35"/>
       <c r="D21" s="38"/>
-      <c r="E21" s="84" t="s">
+      <c r="E21" s="83" t="s">
         <v>45</v>
       </c>
       <c r="F21" s="38"/>
@@ -2103,10 +2104,10 @@
       <c r="I21" s="38"/>
     </row>
     <row r="22" spans="1:11" s="39" customFormat="1" ht="25.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="81"/>
+      <c r="A22" s="80"/>
       <c r="B22" s="35"/>
       <c r="D22" s="38"/>
-      <c r="E22" s="85" t="s">
+      <c r="E22" s="84" t="s">
         <v>46</v>
       </c>
       <c r="F22" s="38"/>
@@ -2115,11 +2116,11 @@
       <c r="I22" s="38"/>
     </row>
     <row r="23" spans="1:11" s="39" customFormat="1" ht="22.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="81"/>
+      <c r="A23" s="80"/>
       <c r="B23" s="35"/>
-      <c r="C23" s="80"/>
+      <c r="C23" s="79"/>
       <c r="D23" s="38"/>
-      <c r="E23" s="86" t="s">
+      <c r="E23" s="85" t="s">
         <v>40</v>
       </c>
       <c r="F23" s="38"/>
@@ -2128,7 +2129,7 @@
       <c r="I23" s="38"/>
     </row>
     <row r="24" spans="1:11" s="37" customFormat="1" ht="21.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="81"/>
+      <c r="A24" s="80"/>
       <c r="B24" s="40"/>
       <c r="C24" s="34"/>
       <c r="D24" s="34"/>
@@ -2139,7 +2140,7 @@
       <c r="I24" s="34"/>
     </row>
     <row r="25" spans="1:11" s="37" customFormat="1" ht="21" x14ac:dyDescent="0.25">
-      <c r="A25" s="81"/>
+      <c r="A25" s="80"/>
       <c r="B25" s="40"/>
       <c r="C25" s="34"/>
       <c r="D25" s="34"/>
@@ -2150,7 +2151,7 @@
       <c r="I25" s="34"/>
     </row>
     <row r="26" spans="1:11" s="39" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="81"/>
+      <c r="A26" s="80"/>
       <c r="B26" s="35"/>
       <c r="C26" s="38"/>
       <c r="D26" s="38"/>
@@ -2161,19 +2162,19 @@
       <c r="I26" s="38"/>
     </row>
     <row r="27" spans="1:11" s="36" customFormat="1" ht="57.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="97" t="str">
+      <c r="A27" s="94" t="str">
         <f>A1</f>
         <v>CS320: SW Engineering - Spring 2018 Schedule
 (as of 3-6-2018, subject to change)</v>
       </c>
-      <c r="B27" s="98"/>
-      <c r="C27" s="98"/>
-      <c r="D27" s="98"/>
-      <c r="E27" s="98"/>
-      <c r="F27" s="98"/>
-      <c r="G27" s="98"/>
-      <c r="H27" s="98"/>
-      <c r="I27" s="99"/>
+      <c r="B27" s="95"/>
+      <c r="C27" s="95"/>
+      <c r="D27" s="95"/>
+      <c r="E27" s="95"/>
+      <c r="F27" s="95"/>
+      <c r="G27" s="95"/>
+      <c r="H27" s="95"/>
+      <c r="I27" s="96"/>
     </row>
     <row r="28" spans="1:11" s="2" customFormat="1" ht="17.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="str">
@@ -2214,79 +2215,79 @@
       </c>
     </row>
     <row r="29" spans="1:11" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="106">
+      <c r="A29" s="97">
         <v>10</v>
       </c>
-      <c r="B29" s="107" t="s">
+      <c r="B29" s="100" t="s">
         <v>43</v>
       </c>
-      <c r="C29" s="64">
+      <c r="C29" s="63">
         <f>C15</f>
         <v>25</v>
       </c>
-      <c r="D29" s="65">
+      <c r="D29" s="64">
         <f>C29 + 1</f>
         <v>26</v>
       </c>
-      <c r="E29" s="68">
+      <c r="E29" s="67">
         <f t="shared" ref="E29" si="4">D29 + 1</f>
         <v>27</v>
       </c>
-      <c r="F29" s="70">
+      <c r="F29" s="69">
         <f>F15</f>
         <v>28</v>
       </c>
-      <c r="G29" s="76">
+      <c r="G29" s="75">
         <v>1</v>
       </c>
-      <c r="H29" s="67">
+      <c r="H29" s="66">
         <f>G29 + 1</f>
         <v>2</v>
       </c>
-      <c r="I29" s="70">
+      <c r="I29" s="69">
         <f>H29 + 1</f>
         <v>3</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="96"/>
-      <c r="B30" s="108"/>
-      <c r="C30" s="77" t="s">
+      <c r="A30" s="98"/>
+      <c r="B30" s="101"/>
+      <c r="C30" s="76" t="s">
         <v>41</v>
       </c>
-      <c r="D30" s="75" t="str">
+      <c r="D30" s="74" t="str">
         <f t="shared" ref="D30" si="5">C30</f>
         <v>WINTER BREAK</v>
       </c>
-      <c r="E30" s="73" t="str">
+      <c r="E30" s="72" t="str">
         <f t="shared" ref="E30" si="6">D30</f>
         <v>WINTER BREAK</v>
       </c>
-      <c r="F30" s="74" t="str">
+      <c r="F30" s="73" t="str">
         <f>E30</f>
         <v>WINTER BREAK</v>
       </c>
-      <c r="G30" s="78" t="str">
+      <c r="G30" s="77" t="str">
         <f>F30</f>
         <v>WINTER BREAK</v>
       </c>
-      <c r="H30" s="65" t="str">
+      <c r="H30" s="64" t="str">
         <f>G30</f>
         <v>WINTER BREAK</v>
       </c>
-      <c r="I30" s="69" t="str">
+      <c r="I30" s="68" t="str">
         <f t="shared" ref="I30" si="7">H30</f>
         <v>WINTER BREAK</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="100">
+      <c r="A31" s="99">
         <v>9</v>
       </c>
-      <c r="B31" s="101" t="s">
+      <c r="B31" s="102" t="s">
         <v>15</v>
       </c>
-      <c r="C31" s="64">
+      <c r="C31" s="63">
         <f>I15 + 1</f>
         <v>4</v>
       </c>
@@ -2316,9 +2317,9 @@
       </c>
     </row>
     <row r="32" spans="1:11" ht="86.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="93"/>
-      <c r="B32" s="109"/>
-      <c r="C32" s="64" t="str">
+      <c r="A32" s="92"/>
+      <c r="B32" s="103"/>
+      <c r="C32" s="63" t="str">
         <f>I30</f>
         <v>WINTER BREAK</v>
       </c>
@@ -2329,22 +2330,22 @@
       <c r="F32" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="G32" s="61" t="s">
+      <c r="G32" s="60" t="s">
         <v>24</v>
       </c>
       <c r="H32" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="I32" s="61" t="s">
+      <c r="I32" s="60" t="s">
         <v>23</v>
       </c>
       <c r="K32" s="43"/>
     </row>
     <row r="33" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="93">
+      <c r="A33" s="92">
         <v>8</v>
       </c>
-      <c r="B33" s="109"/>
+      <c r="B33" s="103"/>
       <c r="C33" s="28">
         <f>I31 + 1</f>
         <v>11</v>
@@ -2375,10 +2376,10 @@
       </c>
     </row>
     <row r="34" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="93"/>
-      <c r="B34" s="109"/>
+      <c r="A34" s="92"/>
+      <c r="B34" s="103"/>
       <c r="C34" s="10"/>
-      <c r="D34" s="45" t="s">
+      <c r="D34" s="44" t="s">
         <v>55</v>
       </c>
       <c r="E34" s="7"/>
@@ -2389,16 +2390,16 @@
       <c r="H34" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="I34" s="62" t="s">
+      <c r="I34" s="61" t="s">
         <v>25</v>
       </c>
       <c r="K34" s="41"/>
     </row>
     <row r="35" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="93">
+      <c r="A35" s="92">
         <v>7</v>
       </c>
-      <c r="B35" s="109"/>
+      <c r="B35" s="103"/>
       <c r="C35" s="10">
         <f>I33 + 1</f>
         <v>18</v>
@@ -2428,28 +2429,28 @@
         <v>24</v>
       </c>
     </row>
-    <row r="36" spans="1:11" ht="54" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="93"/>
-      <c r="B36" s="109"/>
+    <row r="36" spans="1:11" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="92"/>
+      <c r="B36" s="103"/>
       <c r="C36" s="10"/>
       <c r="D36" s="32" t="s">
         <v>18</v>
       </c>
       <c r="E36" s="8"/>
       <c r="F36" s="7" t="s">
-        <v>32</v>
+        <v>74</v>
       </c>
       <c r="G36" s="7"/>
       <c r="H36" s="7" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="I36" s="11"/>
     </row>
     <row r="37" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="93">
+      <c r="A37" s="92">
         <v>6</v>
       </c>
-      <c r="B37" s="109"/>
+      <c r="B37" s="103"/>
       <c r="C37" s="10">
         <f>I35 + 1</f>
         <v>25</v>
@@ -2466,51 +2467,51 @@
         <f t="shared" si="10"/>
         <v>28</v>
       </c>
-      <c r="G37" s="65">
+      <c r="G37" s="64">
         <f t="shared" si="10"/>
         <v>29</v>
       </c>
-      <c r="H37" s="68">
+      <c r="H37" s="67">
         <f t="shared" si="10"/>
         <v>30</v>
       </c>
-      <c r="I37" s="69">
+      <c r="I37" s="68">
         <f>H37 + 1</f>
         <v>31</v>
       </c>
     </row>
-    <row r="38" spans="1:11" ht="44.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="94"/>
-      <c r="B38" s="102"/>
+    <row r="38" spans="1:11" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="93"/>
+      <c r="B38" s="104"/>
       <c r="C38" s="29"/>
-      <c r="D38" s="44" t="s">
-        <v>56</v>
+      <c r="D38" s="14" t="s">
+        <v>19</v>
       </c>
       <c r="E38" s="30"/>
-      <c r="F38" s="56" t="s">
+      <c r="F38" s="55" t="s">
         <v>17</v>
       </c>
-      <c r="G38" s="75" t="s">
+      <c r="G38" s="74" t="s">
         <v>6</v>
       </c>
-      <c r="H38" s="73" t="s">
+      <c r="H38" s="72" t="s">
         <v>6</v>
       </c>
-      <c r="I38" s="74" t="s">
+      <c r="I38" s="73" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="39" spans="1:11" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="100">
+      <c r="A39" s="99">
         <v>5</v>
       </c>
-      <c r="B39" s="103" t="s">
+      <c r="B39" s="109" t="s">
         <v>16</v>
       </c>
-      <c r="C39" s="64">
+      <c r="C39" s="63">
         <v>1</v>
       </c>
-      <c r="D39" s="79">
+      <c r="D39" s="78">
         <f>C39 + 1</f>
         <v>2</v>
       </c>
@@ -2530,37 +2531,37 @@
         <f t="shared" si="11"/>
         <v>6</v>
       </c>
-      <c r="I39" s="50">
+      <c r="I39" s="49">
         <f t="shared" si="11"/>
         <v>7</v>
       </c>
     </row>
     <row r="40" spans="1:11" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="93"/>
-      <c r="B40" s="104"/>
-      <c r="C40" s="64" t="s">
+      <c r="A40" s="92"/>
+      <c r="B40" s="110"/>
+      <c r="C40" s="63" t="s">
         <v>6</v>
       </c>
-      <c r="D40" s="65" t="s">
+      <c r="D40" s="64" t="s">
         <v>6</v>
       </c>
       <c r="E40" s="31"/>
-      <c r="F40" s="31" t="s">
-        <v>7</v>
+      <c r="F40" s="44" t="s">
+        <v>56</v>
       </c>
       <c r="G40" s="17"/>
-      <c r="H40" s="88" t="s">
+      <c r="H40" s="87" t="s">
         <v>51</v>
       </c>
-      <c r="I40" s="62" t="s">
+      <c r="I40" s="61" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="41" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="93">
+      <c r="A41" s="92">
         <v>4</v>
       </c>
-      <c r="B41" s="104"/>
+      <c r="B41" s="110"/>
       <c r="C41" s="24">
         <f>I39 + 1</f>
         <v>8</v>
@@ -2573,50 +2574,50 @@
         <f t="shared" ref="E41:I41" si="12">D41 + 1</f>
         <v>10</v>
       </c>
-      <c r="F41" s="18">
+      <c r="F41" s="21">
         <f t="shared" si="12"/>
         <v>11</v>
       </c>
-      <c r="G41" s="53">
+      <c r="G41" s="52">
         <f t="shared" si="12"/>
         <v>12</v>
       </c>
-      <c r="H41" s="53">
+      <c r="H41" s="52">
         <f t="shared" si="12"/>
         <v>13</v>
       </c>
-      <c r="I41" s="54">
+      <c r="I41" s="53">
         <f t="shared" si="12"/>
         <v>14</v>
       </c>
     </row>
     <row r="42" spans="1:11" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="93"/>
-      <c r="B42" s="104"/>
-      <c r="C42" s="87"/>
-      <c r="D42" s="45" t="s">
+      <c r="A42" s="92"/>
+      <c r="B42" s="110"/>
+      <c r="C42" s="86"/>
+      <c r="D42" s="44" t="s">
         <v>57</v>
       </c>
       <c r="E42" s="17"/>
       <c r="F42" s="31" t="s">
         <v>73</v>
       </c>
-      <c r="G42" s="53"/>
+      <c r="G42" s="52"/>
       <c r="H42" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="I42" s="54"/>
+      <c r="I42" s="53"/>
     </row>
     <row r="43" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="93">
+      <c r="A43" s="92">
         <v>3</v>
       </c>
-      <c r="B43" s="104"/>
-      <c r="C43" s="59">
+      <c r="B43" s="110"/>
+      <c r="C43" s="58">
         <f>I41 + 1</f>
         <v>15</v>
       </c>
-      <c r="D43" s="53">
+      <c r="D43" s="52">
         <f>C43 + 1</f>
         <v>16</v>
       </c>
@@ -2642,9 +2643,9 @@
       </c>
     </row>
     <row r="44" spans="1:11" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="93"/>
-      <c r="B44" s="104"/>
-      <c r="C44" s="57"/>
+      <c r="A44" s="92"/>
+      <c r="B44" s="110"/>
+      <c r="C44" s="56"/>
       <c r="D44" s="32" t="s">
         <v>53</v>
       </c>
@@ -2659,10 +2660,10 @@
       <c r="I44" s="19"/>
     </row>
     <row r="45" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="93">
+      <c r="A45" s="92">
         <v>2</v>
       </c>
-      <c r="B45" s="104"/>
+      <c r="B45" s="110"/>
       <c r="C45" s="24">
         <f>I43 + 1</f>
         <v>22</v>
@@ -2693,13 +2694,13 @@
       </c>
     </row>
     <row r="46" spans="1:11" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="93"/>
-      <c r="B46" s="104"/>
+      <c r="A46" s="92"/>
+      <c r="B46" s="110"/>
       <c r="C46" s="23"/>
-      <c r="D46" s="45" t="s">
+      <c r="D46" s="44" t="s">
         <v>58</v>
       </c>
-      <c r="E46" s="61" t="s">
+      <c r="E46" s="60" t="s">
         <v>59</v>
       </c>
       <c r="F46" s="31" t="s">
@@ -2712,20 +2713,20 @@
       <c r="I46" s="19"/>
     </row>
     <row r="47" spans="1:11" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="93">
+      <c r="A47" s="92">
         <f>A50 + 1</f>
         <v>1</v>
       </c>
-      <c r="B47" s="104"/>
+      <c r="B47" s="110"/>
       <c r="C47" s="24">
         <f>I45 + 1</f>
         <v>29</v>
       </c>
-      <c r="D47" s="49">
+      <c r="D47" s="48">
         <f>C47 + 1</f>
         <v>30</v>
       </c>
-      <c r="E47" s="46">
+      <c r="E47" s="45">
         <v>1</v>
       </c>
       <c r="F47" s="5">
@@ -2746,27 +2747,27 @@
       </c>
     </row>
     <row r="48" spans="1:11" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="94"/>
-      <c r="B48" s="105"/>
-      <c r="C48" s="48"/>
-      <c r="D48" s="58" t="s">
+      <c r="A48" s="93"/>
+      <c r="B48" s="111"/>
+      <c r="C48" s="47"/>
+      <c r="D48" s="57" t="s">
         <v>7</v>
       </c>
-      <c r="E48" s="47"/>
+      <c r="E48" s="46"/>
       <c r="F48" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="G48" s="60"/>
+      <c r="G48" s="59"/>
       <c r="H48" s="8"/>
-      <c r="I48" s="62" t="s">
+      <c r="I48" s="61" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="49" spans="1:9" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="95">
+      <c r="A49" s="108">
         <v>0</v>
       </c>
-      <c r="B49" s="101" t="s">
+      <c r="B49" s="102" t="s">
         <v>5</v>
       </c>
       <c r="C49" s="10">
@@ -2799,11 +2800,11 @@
       </c>
     </row>
     <row r="50" spans="1:9" ht="129.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="96"/>
-      <c r="B50" s="102"/>
+      <c r="A50" s="98"/>
+      <c r="B50" s="104"/>
       <c r="C50" s="14"/>
       <c r="D50" s="14"/>
-      <c r="E50" s="89" t="s">
+      <c r="E50" s="88" t="s">
         <v>34</v>
       </c>
       <c r="F50" s="33" t="s">
@@ -2816,6 +2817,18 @@
     <row r="51" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="A47:A48"/>
+    <mergeCell ref="A49:A50"/>
+    <mergeCell ref="A27:I27"/>
+    <mergeCell ref="A33:A34"/>
+    <mergeCell ref="A35:A36"/>
+    <mergeCell ref="A37:A38"/>
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="A41:A42"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="B39:B48"/>
     <mergeCell ref="A13:A14"/>
     <mergeCell ref="A15:A16"/>
     <mergeCell ref="A1:I1"/>
@@ -2830,18 +2843,6 @@
     <mergeCell ref="B31:B38"/>
     <mergeCell ref="B3:B8"/>
     <mergeCell ref="B9:B16"/>
-    <mergeCell ref="A43:A44"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="A47:A48"/>
-    <mergeCell ref="A49:A50"/>
-    <mergeCell ref="A27:I27"/>
-    <mergeCell ref="A33:A34"/>
-    <mergeCell ref="A35:A36"/>
-    <mergeCell ref="A37:A38"/>
-    <mergeCell ref="A39:A40"/>
-    <mergeCell ref="A41:A42"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="B39:B48"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="5" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
updated schedule to remove IndMS3
</commit_message>
<xml_diff>
--- a/CS320-Spring2018Calendar.xlsx
+++ b/CS320-Spring2018Calendar.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="74">
   <si>
     <t>Monday</t>
   </si>
@@ -287,17 +287,6 @@
     <t>A04: Individual MS1 Baseline Prototype</t>
   </si>
   <si>
-    <t>A04: Individual MS2
-33% Progresss</t>
-  </si>
-  <si>
-    <t>A04: Individual MS3
-67% Progress</t>
-  </si>
-  <si>
-    <t>A04: Individual MS4 Final Project Demo</t>
-  </si>
-  <si>
     <t>A09: Individual Code &amp; Report due
 (Marmoset)</t>
   </si>
@@ -380,8 +369,15 @@
 A SNOW DAY…!</t>
   </si>
   <si>
+    <t>A04: Individual MS2
+50% Progresss</t>
+  </si>
+  <si>
+    <t>A04: Individual MS3 Final Project Demo</t>
+  </si>
+  <si>
     <t>CS320: SW Engineering - Spring 2018 Schedule
-(as of 3-22-2018, subject to change)</t>
+(as of 3-23-2018, subject to change)</t>
   </si>
 </sst>
 </file>
@@ -1234,30 +1230,51 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
@@ -1265,27 +1282,6 @@
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1594,7 +1590,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -1613,17 +1609,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="57.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="96" t="s">
-        <v>74</v>
-      </c>
-      <c r="B1" s="97"/>
-      <c r="C1" s="97"/>
-      <c r="D1" s="97"/>
-      <c r="E1" s="97"/>
-      <c r="F1" s="97"/>
-      <c r="G1" s="97"/>
-      <c r="H1" s="97"/>
-      <c r="I1" s="98"/>
+      <c r="A1" s="94" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" s="95"/>
+      <c r="C1" s="95"/>
+      <c r="D1" s="95"/>
+      <c r="E1" s="95"/>
+      <c r="F1" s="95"/>
+      <c r="G1" s="95"/>
+      <c r="H1" s="95"/>
+      <c r="I1" s="96"/>
     </row>
     <row r="2" spans="1:13" s="2" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -1656,7 +1652,7 @@
       <c r="A3" s="99">
         <v>16</v>
       </c>
-      <c r="B3" s="100" t="s">
+      <c r="B3" s="102" t="s">
         <v>13</v>
       </c>
       <c r="C3" s="65">
@@ -1689,7 +1685,7 @@
     </row>
     <row r="4" spans="1:13" ht="81.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="92"/>
-      <c r="B4" s="108"/>
+      <c r="B4" s="103"/>
       <c r="C4" s="63" t="s">
         <v>10</v>
       </c>
@@ -1712,7 +1708,7 @@
       <c r="A5" s="92">
         <v>15</v>
       </c>
-      <c r="B5" s="108"/>
+      <c r="B5" s="103"/>
       <c r="C5" s="10">
         <f>I3 + 1</f>
         <v>21</v>
@@ -1744,22 +1740,22 @@
     </row>
     <row r="6" spans="1:13" ht="82.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="92"/>
-      <c r="B6" s="108"/>
+      <c r="B6" s="103"/>
       <c r="C6" s="62" t="s">
         <v>9</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E6" s="8"/>
       <c r="F6" s="7" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="G6" s="60" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="I6" s="91"/>
     </row>
@@ -1767,7 +1763,7 @@
       <c r="A7" s="92">
         <v>14</v>
       </c>
-      <c r="B7" s="108"/>
+      <c r="B7" s="103"/>
       <c r="C7" s="10">
         <f>I5 + 1</f>
         <v>28</v>
@@ -1798,7 +1794,7 @@
     </row>
     <row r="8" spans="1:13" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="93"/>
-      <c r="B8" s="101"/>
+      <c r="B8" s="104"/>
       <c r="C8" s="89" t="s">
         <v>20</v>
       </c>
@@ -1807,11 +1803,11 @@
       </c>
       <c r="E8" s="30"/>
       <c r="F8" s="54" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="G8" s="17"/>
       <c r="H8" s="16" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="I8" s="61" t="s">
         <v>26</v>
@@ -1821,7 +1817,7 @@
       <c r="A9" s="99">
         <v>13</v>
       </c>
-      <c r="B9" s="109" t="s">
+      <c r="B9" s="105" t="s">
         <v>14</v>
       </c>
       <c r="C9" s="20">
@@ -1855,16 +1851,16 @@
     </row>
     <row r="10" spans="1:13" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="92"/>
-      <c r="B10" s="110"/>
+      <c r="B10" s="106"/>
       <c r="C10" s="62" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D10" s="18" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E10" s="17"/>
       <c r="F10" s="18" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="G10" s="17"/>
       <c r="H10" s="18" t="s">
@@ -1876,7 +1872,7 @@
       <c r="A11" s="92">
         <v>12</v>
       </c>
-      <c r="B11" s="110"/>
+      <c r="B11" s="106"/>
       <c r="C11" s="24">
         <f>I9 + 1</f>
         <v>11</v>
@@ -1908,20 +1904,20 @@
     </row>
     <row r="12" spans="1:13" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="92"/>
-      <c r="B12" s="110"/>
+      <c r="B12" s="106"/>
       <c r="C12" s="62" t="s">
         <v>54</v>
       </c>
       <c r="D12" s="18" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E12" s="17"/>
       <c r="F12" s="18" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="G12" s="17"/>
       <c r="H12" s="18" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="I12" s="19"/>
     </row>
@@ -1929,7 +1925,7 @@
       <c r="A13" s="92">
         <v>11</v>
       </c>
-      <c r="B13" s="110"/>
+      <c r="B13" s="106"/>
       <c r="C13" s="24">
         <f>I11 + 1</f>
         <v>18</v>
@@ -1961,7 +1957,7 @@
     </row>
     <row r="14" spans="1:13" ht="83.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="92"/>
-      <c r="B14" s="110"/>
+      <c r="B14" s="106"/>
       <c r="C14" s="24"/>
       <c r="D14" s="18" t="s">
         <v>28</v>
@@ -1984,7 +1980,7 @@
       <c r="A15" s="92">
         <v>10</v>
       </c>
-      <c r="B15" s="110"/>
+      <c r="B15" s="106"/>
       <c r="C15" s="63">
         <f>I13 + 1</f>
         <v>25</v>
@@ -2015,7 +2011,7 @@
     </row>
     <row r="16" spans="1:13" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="93"/>
-      <c r="B16" s="111"/>
+      <c r="B16" s="107"/>
       <c r="C16" s="70" t="s">
         <v>41</v>
       </c>
@@ -2162,19 +2158,19 @@
       <c r="I26" s="38"/>
     </row>
     <row r="27" spans="1:11" s="36" customFormat="1" ht="57.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="96" t="str">
+      <c r="A27" s="94" t="str">
         <f>A1</f>
         <v>CS320: SW Engineering - Spring 2018 Schedule
-(as of 3-22-2018, subject to change)</v>
-      </c>
-      <c r="B27" s="97"/>
-      <c r="C27" s="97"/>
-      <c r="D27" s="97"/>
-      <c r="E27" s="97"/>
-      <c r="F27" s="97"/>
-      <c r="G27" s="97"/>
-      <c r="H27" s="97"/>
-      <c r="I27" s="98"/>
+(as of 3-23-2018, subject to change)</v>
+      </c>
+      <c r="B27" s="95"/>
+      <c r="C27" s="95"/>
+      <c r="D27" s="95"/>
+      <c r="E27" s="95"/>
+      <c r="F27" s="95"/>
+      <c r="G27" s="95"/>
+      <c r="H27" s="95"/>
+      <c r="I27" s="96"/>
     </row>
     <row r="28" spans="1:11" s="2" customFormat="1" ht="17.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="str">
@@ -2215,10 +2211,10 @@
       </c>
     </row>
     <row r="29" spans="1:11" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="105">
+      <c r="A29" s="97">
         <v>10</v>
       </c>
-      <c r="B29" s="106" t="s">
+      <c r="B29" s="100" t="s">
         <v>43</v>
       </c>
       <c r="C29" s="63">
@@ -2250,8 +2246,8 @@
       </c>
     </row>
     <row r="30" spans="1:11" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="95"/>
-      <c r="B30" s="107"/>
+      <c r="A30" s="98"/>
+      <c r="B30" s="101"/>
       <c r="C30" s="76" t="s">
         <v>41</v>
       </c>
@@ -2284,7 +2280,7 @@
       <c r="A31" s="99">
         <v>9</v>
       </c>
-      <c r="B31" s="100" t="s">
+      <c r="B31" s="102" t="s">
         <v>15</v>
       </c>
       <c r="C31" s="63">
@@ -2318,7 +2314,7 @@
     </row>
     <row r="32" spans="1:11" ht="86.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="92"/>
-      <c r="B32" s="108"/>
+      <c r="B32" s="103"/>
       <c r="C32" s="63" t="str">
         <f>I30</f>
         <v>WINTER BREAK</v>
@@ -2345,7 +2341,7 @@
       <c r="A33" s="92">
         <v>8</v>
       </c>
-      <c r="B33" s="108"/>
+      <c r="B33" s="103"/>
       <c r="C33" s="28">
         <f>I31 + 1</f>
         <v>11</v>
@@ -2377,7 +2373,7 @@
     </row>
     <row r="34" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="92"/>
-      <c r="B34" s="108"/>
+      <c r="B34" s="103"/>
       <c r="C34" s="10"/>
       <c r="D34" s="44" t="s">
         <v>55</v>
@@ -2399,7 +2395,7 @@
       <c r="A35" s="92">
         <v>7</v>
       </c>
-      <c r="B35" s="108"/>
+      <c r="B35" s="103"/>
       <c r="C35" s="10">
         <f>I33 + 1</f>
         <v>18</v>
@@ -2431,14 +2427,14 @@
     </row>
     <row r="36" spans="1:11" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="92"/>
-      <c r="B36" s="108"/>
+      <c r="B36" s="103"/>
       <c r="C36" s="10"/>
       <c r="D36" s="32" t="s">
         <v>18</v>
       </c>
       <c r="E36" s="8"/>
       <c r="F36" s="7" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="G36" s="7"/>
       <c r="H36" s="7" t="s">
@@ -2450,7 +2446,7 @@
       <c r="A37" s="92">
         <v>6</v>
       </c>
-      <c r="B37" s="108"/>
+      <c r="B37" s="103"/>
       <c r="C37" s="10">
         <f>I35 + 1</f>
         <v>25</v>
@@ -2482,7 +2478,7 @@
     </row>
     <row r="38" spans="1:11" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="93"/>
-      <c r="B38" s="101"/>
+      <c r="B38" s="104"/>
       <c r="C38" s="29"/>
       <c r="D38" s="14" t="s">
         <v>19</v>
@@ -2505,7 +2501,7 @@
       <c r="A39" s="99">
         <v>5</v>
       </c>
-      <c r="B39" s="102" t="s">
+      <c r="B39" s="109" t="s">
         <v>16</v>
       </c>
       <c r="C39" s="63">
@@ -2538,7 +2534,7 @@
     </row>
     <row r="40" spans="1:11" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="92"/>
-      <c r="B40" s="103"/>
+      <c r="B40" s="110"/>
       <c r="C40" s="63" t="s">
         <v>6</v>
       </c>
@@ -2547,7 +2543,7 @@
       </c>
       <c r="E40" s="31"/>
       <c r="F40" s="44" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="G40" s="17"/>
       <c r="H40" s="87" t="s">
@@ -2561,7 +2557,7 @@
       <c r="A41" s="92">
         <v>4</v>
       </c>
-      <c r="B41" s="103"/>
+      <c r="B41" s="110"/>
       <c r="C41" s="24">
         <f>I39 + 1</f>
         <v>8</v>
@@ -2593,14 +2589,14 @@
     </row>
     <row r="42" spans="1:11" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="92"/>
-      <c r="B42" s="103"/>
+      <c r="B42" s="110"/>
       <c r="C42" s="86"/>
-      <c r="D42" s="44" t="s">
-        <v>57</v>
+      <c r="D42" s="31" t="s">
+        <v>7</v>
       </c>
       <c r="E42" s="17"/>
       <c r="F42" s="31" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="G42" s="52"/>
       <c r="H42" s="31" t="s">
@@ -2612,7 +2608,7 @@
       <c r="A43" s="92">
         <v>3</v>
       </c>
-      <c r="B43" s="103"/>
+      <c r="B43" s="110"/>
       <c r="C43" s="58">
         <f>I41 + 1</f>
         <v>15</v>
@@ -2644,7 +2640,7 @@
     </row>
     <row r="44" spans="1:11" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="92"/>
-      <c r="B44" s="103"/>
+      <c r="B44" s="110"/>
       <c r="C44" s="56"/>
       <c r="D44" s="32" t="s">
         <v>53</v>
@@ -2663,7 +2659,7 @@
       <c r="A45" s="92">
         <v>2</v>
       </c>
-      <c r="B45" s="103"/>
+      <c r="B45" s="110"/>
       <c r="C45" s="24">
         <f>I43 + 1</f>
         <v>22</v>
@@ -2695,13 +2691,13 @@
     </row>
     <row r="46" spans="1:11" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="92"/>
-      <c r="B46" s="103"/>
+      <c r="B46" s="110"/>
       <c r="C46" s="23"/>
       <c r="D46" s="44" t="s">
-        <v>58</v>
+        <v>72</v>
       </c>
       <c r="E46" s="60" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="F46" s="31" t="s">
         <v>7</v>
@@ -2717,7 +2713,7 @@
         <f>A50 + 1</f>
         <v>1</v>
       </c>
-      <c r="B47" s="103"/>
+      <c r="B47" s="110"/>
       <c r="C47" s="24">
         <f>I45 + 1</f>
         <v>29</v>
@@ -2748,7 +2744,7 @@
     </row>
     <row r="48" spans="1:11" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="93"/>
-      <c r="B48" s="104"/>
+      <c r="B48" s="111"/>
       <c r="C48" s="47"/>
       <c r="D48" s="57" t="s">
         <v>7</v>
@@ -2764,10 +2760,10 @@
       </c>
     </row>
     <row r="49" spans="1:9" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="94">
+      <c r="A49" s="108">
         <v>0</v>
       </c>
-      <c r="B49" s="100" t="s">
+      <c r="B49" s="102" t="s">
         <v>5</v>
       </c>
       <c r="C49" s="10">
@@ -2800,8 +2796,8 @@
       </c>
     </row>
     <row r="50" spans="1:9" ht="129.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="95"/>
-      <c r="B50" s="101"/>
+      <c r="A50" s="98"/>
+      <c r="B50" s="104"/>
       <c r="C50" s="14"/>
       <c r="D50" s="14"/>
       <c r="E50" s="88" t="s">
@@ -2817,6 +2813,18 @@
     <row r="51" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="A47:A48"/>
+    <mergeCell ref="A49:A50"/>
+    <mergeCell ref="A27:I27"/>
+    <mergeCell ref="A33:A34"/>
+    <mergeCell ref="A35:A36"/>
+    <mergeCell ref="A37:A38"/>
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="A41:A42"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="B39:B48"/>
     <mergeCell ref="A13:A14"/>
     <mergeCell ref="A15:A16"/>
     <mergeCell ref="A1:I1"/>
@@ -2831,18 +2839,6 @@
     <mergeCell ref="B31:B38"/>
     <mergeCell ref="B3:B8"/>
     <mergeCell ref="B9:B16"/>
-    <mergeCell ref="A43:A44"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="A47:A48"/>
-    <mergeCell ref="A49:A50"/>
-    <mergeCell ref="A27:I27"/>
-    <mergeCell ref="A33:A34"/>
-    <mergeCell ref="A35:A36"/>
-    <mergeCell ref="A37:A38"/>
-    <mergeCell ref="A39:A40"/>
-    <mergeCell ref="A41:A42"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="B39:B48"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="5" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
updates for peer evals
</commit_message>
<xml_diff>
--- a/CS320-Spring2018Calendar.xlsx
+++ b/CS320-Spring2018Calendar.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\djhake2\cs320-spring2018\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="90" yWindow="-165" windowWidth="15825" windowHeight="12075"/>
   </bookViews>
@@ -11,7 +16,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -377,7 +382,7 @@
   </si>
   <si>
     <t>CS320: SW Engineering - Spring 2018 Schedule
-(as of 3-23-2018, subject to change)</t>
+(as of 4-6-2018, subject to change)</t>
   </si>
 </sst>
 </file>
@@ -1206,9 +1211,6 @@
     <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1230,6 +1232,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1239,13 +1247,25 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1254,15 +1274,9 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
@@ -1272,17 +1286,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1344,7 +1349,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1379,7 +1384,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1590,8 +1595,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41:A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1609,17 +1614,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="57.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="94" t="s">
+      <c r="A1" s="95" t="s">
         <v>73</v>
       </c>
-      <c r="B1" s="95"/>
-      <c r="C1" s="95"/>
-      <c r="D1" s="95"/>
-      <c r="E1" s="95"/>
-      <c r="F1" s="95"/>
-      <c r="G1" s="95"/>
-      <c r="H1" s="95"/>
-      <c r="I1" s="96"/>
+      <c r="B1" s="96"/>
+      <c r="C1" s="96"/>
+      <c r="D1" s="96"/>
+      <c r="E1" s="96"/>
+      <c r="F1" s="96"/>
+      <c r="G1" s="96"/>
+      <c r="H1" s="96"/>
+      <c r="I1" s="97"/>
     </row>
     <row r="2" spans="1:13" s="2" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -1649,10 +1654,10 @@
       </c>
     </row>
     <row r="3" spans="1:13" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="99">
+      <c r="A3" s="98">
         <v>16</v>
       </c>
-      <c r="B3" s="102" t="s">
+      <c r="B3" s="99" t="s">
         <v>13</v>
       </c>
       <c r="C3" s="65">
@@ -1684,8 +1689,8 @@
       </c>
     </row>
     <row r="4" spans="1:13" ht="81.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="92"/>
-      <c r="B4" s="103"/>
+      <c r="A4" s="91"/>
+      <c r="B4" s="107"/>
       <c r="C4" s="63" t="s">
         <v>10</v>
       </c>
@@ -1705,10 +1710,10 @@
       <c r="I4" s="9"/>
     </row>
     <row r="5" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="92">
+      <c r="A5" s="91">
         <v>15</v>
       </c>
-      <c r="B5" s="103"/>
+      <c r="B5" s="107"/>
       <c r="C5" s="10">
         <f>I3 + 1</f>
         <v>21</v>
@@ -1739,8 +1744,8 @@
       </c>
     </row>
     <row r="6" spans="1:13" ht="82.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="92"/>
-      <c r="B6" s="103"/>
+      <c r="A6" s="91"/>
+      <c r="B6" s="107"/>
       <c r="C6" s="62" t="s">
         <v>9</v>
       </c>
@@ -1757,13 +1762,13 @@
       <c r="H6" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="I6" s="91"/>
+      <c r="I6" s="90"/>
     </row>
     <row r="7" spans="1:13" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="92">
+      <c r="A7" s="91">
         <v>14</v>
       </c>
-      <c r="B7" s="103"/>
+      <c r="B7" s="107"/>
       <c r="C7" s="10">
         <f>I5 + 1</f>
         <v>28</v>
@@ -1793,9 +1798,9 @@
       </c>
     </row>
     <row r="8" spans="1:13" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="93"/>
-      <c r="B8" s="104"/>
-      <c r="C8" s="89" t="s">
+      <c r="A8" s="92"/>
+      <c r="B8" s="100"/>
+      <c r="C8" s="88" t="s">
         <v>20</v>
       </c>
       <c r="D8" s="14" t="s">
@@ -1814,10 +1819,10 @@
       </c>
     </row>
     <row r="9" spans="1:13" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="99">
+      <c r="A9" s="98">
         <v>13</v>
       </c>
-      <c r="B9" s="105" t="s">
+      <c r="B9" s="108" t="s">
         <v>14</v>
       </c>
       <c r="C9" s="20">
@@ -1850,8 +1855,8 @@
       </c>
     </row>
     <row r="10" spans="1:13" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="92"/>
-      <c r="B10" s="106"/>
+      <c r="A10" s="91"/>
+      <c r="B10" s="109"/>
       <c r="C10" s="62" t="s">
         <v>58</v>
       </c>
@@ -1869,10 +1874,10 @@
       <c r="I10" s="19"/>
     </row>
     <row r="11" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="92">
+      <c r="A11" s="91">
         <v>12</v>
       </c>
-      <c r="B11" s="106"/>
+      <c r="B11" s="109"/>
       <c r="C11" s="24">
         <f>I9 + 1</f>
         <v>11</v>
@@ -1903,8 +1908,8 @@
       </c>
     </row>
     <row r="12" spans="1:13" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="92"/>
-      <c r="B12" s="106"/>
+      <c r="A12" s="91"/>
+      <c r="B12" s="109"/>
       <c r="C12" s="62" t="s">
         <v>54</v>
       </c>
@@ -1922,10 +1927,10 @@
       <c r="I12" s="19"/>
     </row>
     <row r="13" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="92">
+      <c r="A13" s="91">
         <v>11</v>
       </c>
-      <c r="B13" s="106"/>
+      <c r="B13" s="109"/>
       <c r="C13" s="24">
         <f>I11 + 1</f>
         <v>18</v>
@@ -1956,8 +1961,8 @@
       </c>
     </row>
     <row r="14" spans="1:13" ht="83.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="92"/>
-      <c r="B14" s="106"/>
+      <c r="A14" s="91"/>
+      <c r="B14" s="109"/>
       <c r="C14" s="24"/>
       <c r="D14" s="18" t="s">
         <v>28</v>
@@ -1977,10 +1982,10 @@
       <c r="M14" s="42"/>
     </row>
     <row r="15" spans="1:13" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="92">
+      <c r="A15" s="91">
         <v>10</v>
       </c>
-      <c r="B15" s="106"/>
+      <c r="B15" s="109"/>
       <c r="C15" s="63">
         <f>I13 + 1</f>
         <v>25</v>
@@ -2010,8 +2015,8 @@
       </c>
     </row>
     <row r="16" spans="1:13" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="93"/>
-      <c r="B16" s="107"/>
+      <c r="A16" s="92"/>
+      <c r="B16" s="110"/>
       <c r="C16" s="70" t="s">
         <v>41</v>
       </c>
@@ -2055,7 +2060,7 @@
       <c r="A18" s="80"/>
       <c r="B18" s="35"/>
       <c r="D18" s="38"/>
-      <c r="E18" s="90" t="s">
+      <c r="E18" s="89" t="s">
         <v>50</v>
       </c>
       <c r="F18" s="38"/>
@@ -2158,19 +2163,19 @@
       <c r="I26" s="38"/>
     </row>
     <row r="27" spans="1:11" s="36" customFormat="1" ht="57.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="94" t="str">
+      <c r="A27" s="95" t="str">
         <f>A1</f>
         <v>CS320: SW Engineering - Spring 2018 Schedule
-(as of 3-23-2018, subject to change)</v>
-      </c>
-      <c r="B27" s="95"/>
-      <c r="C27" s="95"/>
-      <c r="D27" s="95"/>
-      <c r="E27" s="95"/>
-      <c r="F27" s="95"/>
-      <c r="G27" s="95"/>
-      <c r="H27" s="95"/>
-      <c r="I27" s="96"/>
+(as of 4-6-2018, subject to change)</v>
+      </c>
+      <c r="B27" s="96"/>
+      <c r="C27" s="96"/>
+      <c r="D27" s="96"/>
+      <c r="E27" s="96"/>
+      <c r="F27" s="96"/>
+      <c r="G27" s="96"/>
+      <c r="H27" s="96"/>
+      <c r="I27" s="97"/>
     </row>
     <row r="28" spans="1:11" s="2" customFormat="1" ht="17.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="str">
@@ -2211,10 +2216,10 @@
       </c>
     </row>
     <row r="29" spans="1:11" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="97">
+      <c r="A29" s="104">
         <v>10</v>
       </c>
-      <c r="B29" s="100" t="s">
+      <c r="B29" s="105" t="s">
         <v>43</v>
       </c>
       <c r="C29" s="63">
@@ -2246,8 +2251,8 @@
       </c>
     </row>
     <row r="30" spans="1:11" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="98"/>
-      <c r="B30" s="101"/>
+      <c r="A30" s="94"/>
+      <c r="B30" s="106"/>
       <c r="C30" s="76" t="s">
         <v>41</v>
       </c>
@@ -2277,10 +2282,10 @@
       </c>
     </row>
     <row r="31" spans="1:11" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="99">
+      <c r="A31" s="98">
         <v>9</v>
       </c>
-      <c r="B31" s="102" t="s">
+      <c r="B31" s="99" t="s">
         <v>15</v>
       </c>
       <c r="C31" s="63">
@@ -2313,8 +2318,8 @@
       </c>
     </row>
     <row r="32" spans="1:11" ht="86.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="92"/>
-      <c r="B32" s="103"/>
+      <c r="A32" s="91"/>
+      <c r="B32" s="107"/>
       <c r="C32" s="63" t="str">
         <f>I30</f>
         <v>WINTER BREAK</v>
@@ -2338,10 +2343,10 @@
       <c r="K32" s="43"/>
     </row>
     <row r="33" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="92">
+      <c r="A33" s="91">
         <v>8</v>
       </c>
-      <c r="B33" s="103"/>
+      <c r="B33" s="107"/>
       <c r="C33" s="28">
         <f>I31 + 1</f>
         <v>11</v>
@@ -2372,8 +2377,8 @@
       </c>
     </row>
     <row r="34" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="92"/>
-      <c r="B34" s="103"/>
+      <c r="A34" s="91"/>
+      <c r="B34" s="107"/>
       <c r="C34" s="10"/>
       <c r="D34" s="44" t="s">
         <v>55</v>
@@ -2392,10 +2397,10 @@
       <c r="K34" s="41"/>
     </row>
     <row r="35" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="92">
+      <c r="A35" s="91">
         <v>7</v>
       </c>
-      <c r="B35" s="103"/>
+      <c r="B35" s="107"/>
       <c r="C35" s="10">
         <f>I33 + 1</f>
         <v>18</v>
@@ -2426,8 +2431,8 @@
       </c>
     </row>
     <row r="36" spans="1:11" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="92"/>
-      <c r="B36" s="103"/>
+      <c r="A36" s="91"/>
+      <c r="B36" s="107"/>
       <c r="C36" s="10"/>
       <c r="D36" s="32" t="s">
         <v>18</v>
@@ -2443,10 +2448,10 @@
       <c r="I36" s="11"/>
     </row>
     <row r="37" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="92">
+      <c r="A37" s="91">
         <v>6</v>
       </c>
-      <c r="B37" s="103"/>
+      <c r="B37" s="107"/>
       <c r="C37" s="10">
         <f>I35 + 1</f>
         <v>25</v>
@@ -2477,8 +2482,8 @@
       </c>
     </row>
     <row r="38" spans="1:11" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="93"/>
-      <c r="B38" s="104"/>
+      <c r="A38" s="92"/>
+      <c r="B38" s="100"/>
       <c r="C38" s="29"/>
       <c r="D38" s="14" t="s">
         <v>19</v>
@@ -2498,10 +2503,10 @@
       </c>
     </row>
     <row r="39" spans="1:11" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="99">
+      <c r="A39" s="98">
         <v>5</v>
       </c>
-      <c r="B39" s="109" t="s">
+      <c r="B39" s="101" t="s">
         <v>16</v>
       </c>
       <c r="C39" s="63">
@@ -2532,9 +2537,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="40" spans="1:11" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="92"/>
-      <c r="B40" s="110"/>
+    <row r="40" spans="1:11" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="91"/>
+      <c r="B40" s="102"/>
       <c r="C40" s="63" t="s">
         <v>6</v>
       </c>
@@ -2546,18 +2551,16 @@
         <v>71</v>
       </c>
       <c r="G40" s="17"/>
-      <c r="H40" s="87" t="s">
+      <c r="H40" s="86" t="s">
         <v>51</v>
       </c>
-      <c r="I40" s="61" t="s">
-        <v>33</v>
-      </c>
+      <c r="I40" s="111"/>
     </row>
     <row r="41" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="92">
+      <c r="A41" s="91">
         <v>4</v>
       </c>
-      <c r="B41" s="110"/>
+      <c r="B41" s="102"/>
       <c r="C41" s="24">
         <f>I39 + 1</f>
         <v>8</v>
@@ -2587,10 +2590,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="42" spans="1:11" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="92"/>
-      <c r="B42" s="110"/>
-      <c r="C42" s="86"/>
+    <row r="42" spans="1:11" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="91"/>
+      <c r="B42" s="102"/>
+      <c r="C42" s="61" t="s">
+        <v>33</v>
+      </c>
       <c r="D42" s="31" t="s">
         <v>7</v>
       </c>
@@ -2605,10 +2610,10 @@
       <c r="I42" s="53"/>
     </row>
     <row r="43" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="92">
+      <c r="A43" s="91">
         <v>3</v>
       </c>
-      <c r="B43" s="110"/>
+      <c r="B43" s="102"/>
       <c r="C43" s="58">
         <f>I41 + 1</f>
         <v>15</v>
@@ -2638,9 +2643,9 @@
         <v>21</v>
       </c>
     </row>
-    <row r="44" spans="1:11" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="92"/>
-      <c r="B44" s="110"/>
+    <row r="44" spans="1:11" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="91"/>
+      <c r="B44" s="102"/>
       <c r="C44" s="56"/>
       <c r="D44" s="32" t="s">
         <v>53</v>
@@ -2656,10 +2661,10 @@
       <c r="I44" s="19"/>
     </row>
     <row r="45" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="92">
+      <c r="A45" s="91">
         <v>2</v>
       </c>
-      <c r="B45" s="110"/>
+      <c r="B45" s="102"/>
       <c r="C45" s="24">
         <f>I43 + 1</f>
         <v>22</v>
@@ -2690,8 +2695,8 @@
       </c>
     </row>
     <row r="46" spans="1:11" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="92"/>
-      <c r="B46" s="110"/>
+      <c r="A46" s="91"/>
+      <c r="B46" s="102"/>
       <c r="C46" s="23"/>
       <c r="D46" s="44" t="s">
         <v>72</v>
@@ -2709,11 +2714,11 @@
       <c r="I46" s="19"/>
     </row>
     <row r="47" spans="1:11" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="92">
+      <c r="A47" s="91">
         <f>A50 + 1</f>
         <v>1</v>
       </c>
-      <c r="B47" s="110"/>
+      <c r="B47" s="102"/>
       <c r="C47" s="24">
         <f>I45 + 1</f>
         <v>29</v>
@@ -2743,8 +2748,8 @@
       </c>
     </row>
     <row r="48" spans="1:11" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="93"/>
-      <c r="B48" s="111"/>
+      <c r="A48" s="92"/>
+      <c r="B48" s="103"/>
       <c r="C48" s="47"/>
       <c r="D48" s="57" t="s">
         <v>7</v>
@@ -2760,10 +2765,10 @@
       </c>
     </row>
     <row r="49" spans="1:9" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="108">
+      <c r="A49" s="93">
         <v>0</v>
       </c>
-      <c r="B49" s="102" t="s">
+      <c r="B49" s="99" t="s">
         <v>5</v>
       </c>
       <c r="C49" s="10">
@@ -2796,11 +2801,11 @@
       </c>
     </row>
     <row r="50" spans="1:9" ht="129.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="98"/>
-      <c r="B50" s="104"/>
+      <c r="A50" s="94"/>
+      <c r="B50" s="100"/>
       <c r="C50" s="14"/>
       <c r="D50" s="14"/>
-      <c r="E50" s="88" t="s">
+      <c r="E50" s="87" t="s">
         <v>34</v>
       </c>
       <c r="F50" s="33" t="s">
@@ -2813,18 +2818,6 @@
     <row r="51" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="A43:A44"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="A47:A48"/>
-    <mergeCell ref="A49:A50"/>
-    <mergeCell ref="A27:I27"/>
-    <mergeCell ref="A33:A34"/>
-    <mergeCell ref="A35:A36"/>
-    <mergeCell ref="A37:A38"/>
-    <mergeCell ref="A39:A40"/>
-    <mergeCell ref="A41:A42"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="B39:B48"/>
     <mergeCell ref="A13:A14"/>
     <mergeCell ref="A15:A16"/>
     <mergeCell ref="A1:I1"/>
@@ -2839,6 +2832,18 @@
     <mergeCell ref="B31:B38"/>
     <mergeCell ref="B3:B8"/>
     <mergeCell ref="B9:B16"/>
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="A47:A48"/>
+    <mergeCell ref="A49:A50"/>
+    <mergeCell ref="A27:I27"/>
+    <mergeCell ref="A33:A34"/>
+    <mergeCell ref="A35:A36"/>
+    <mergeCell ref="A37:A38"/>
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="A41:A42"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="B39:B48"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="5" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
moved TeamMS3 to 4-20
</commit_message>
<xml_diff>
--- a/CS320-Spring2018Calendar.xlsx
+++ b/CS320-Spring2018Calendar.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\djhake2\cs320-spring2018\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="90" yWindow="-165" windowWidth="15825" windowHeight="12075"/>
   </bookViews>
@@ -16,7 +11,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -382,7 +377,7 @@
   </si>
   <si>
     <t>CS320: SW Engineering - Spring 2018 Schedule
-(as of 4-6-2018, subject to change)</t>
+(as of 4-9-2018, subject to change)</t>
   </si>
 </sst>
 </file>
@@ -954,7 +949,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="112">
+  <cellXfs count="113">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1226,36 +1221,60 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
@@ -1265,28 +1284,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1349,7 +1347,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1384,7 +1382,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1595,8 +1593,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41:A42"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection sqref="A1:I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1614,17 +1612,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="57.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="95" t="s">
+      <c r="A1" s="94" t="s">
         <v>73</v>
       </c>
-      <c r="B1" s="96"/>
-      <c r="C1" s="96"/>
-      <c r="D1" s="96"/>
-      <c r="E1" s="96"/>
-      <c r="F1" s="96"/>
-      <c r="G1" s="96"/>
-      <c r="H1" s="96"/>
-      <c r="I1" s="97"/>
+      <c r="B1" s="95"/>
+      <c r="C1" s="95"/>
+      <c r="D1" s="95"/>
+      <c r="E1" s="95"/>
+      <c r="F1" s="95"/>
+      <c r="G1" s="95"/>
+      <c r="H1" s="95"/>
+      <c r="I1" s="96"/>
     </row>
     <row r="2" spans="1:13" s="2" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -1654,10 +1652,10 @@
       </c>
     </row>
     <row r="3" spans="1:13" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="98">
+      <c r="A3" s="99">
         <v>16</v>
       </c>
-      <c r="B3" s="99" t="s">
+      <c r="B3" s="102" t="s">
         <v>13</v>
       </c>
       <c r="C3" s="65">
@@ -1689,8 +1687,8 @@
       </c>
     </row>
     <row r="4" spans="1:13" ht="81.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="91"/>
-      <c r="B4" s="107"/>
+      <c r="A4" s="92"/>
+      <c r="B4" s="103"/>
       <c r="C4" s="63" t="s">
         <v>10</v>
       </c>
@@ -1710,10 +1708,10 @@
       <c r="I4" s="9"/>
     </row>
     <row r="5" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="91">
+      <c r="A5" s="92">
         <v>15</v>
       </c>
-      <c r="B5" s="107"/>
+      <c r="B5" s="103"/>
       <c r="C5" s="10">
         <f>I3 + 1</f>
         <v>21</v>
@@ -1744,8 +1742,8 @@
       </c>
     </row>
     <row r="6" spans="1:13" ht="82.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="91"/>
-      <c r="B6" s="107"/>
+      <c r="A6" s="92"/>
+      <c r="B6" s="103"/>
       <c r="C6" s="62" t="s">
         <v>9</v>
       </c>
@@ -1765,10 +1763,10 @@
       <c r="I6" s="90"/>
     </row>
     <row r="7" spans="1:13" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="91">
+      <c r="A7" s="92">
         <v>14</v>
       </c>
-      <c r="B7" s="107"/>
+      <c r="B7" s="103"/>
       <c r="C7" s="10">
         <f>I5 + 1</f>
         <v>28</v>
@@ -1798,8 +1796,8 @@
       </c>
     </row>
     <row r="8" spans="1:13" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="92"/>
-      <c r="B8" s="100"/>
+      <c r="A8" s="93"/>
+      <c r="B8" s="104"/>
       <c r="C8" s="88" t="s">
         <v>20</v>
       </c>
@@ -1819,10 +1817,10 @@
       </c>
     </row>
     <row r="9" spans="1:13" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="98">
+      <c r="A9" s="99">
         <v>13</v>
       </c>
-      <c r="B9" s="108" t="s">
+      <c r="B9" s="105" t="s">
         <v>14</v>
       </c>
       <c r="C9" s="20">
@@ -1855,8 +1853,8 @@
       </c>
     </row>
     <row r="10" spans="1:13" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="91"/>
-      <c r="B10" s="109"/>
+      <c r="A10" s="92"/>
+      <c r="B10" s="106"/>
       <c r="C10" s="62" t="s">
         <v>58</v>
       </c>
@@ -1874,10 +1872,10 @@
       <c r="I10" s="19"/>
     </row>
     <row r="11" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="91">
+      <c r="A11" s="92">
         <v>12</v>
       </c>
-      <c r="B11" s="109"/>
+      <c r="B11" s="106"/>
       <c r="C11" s="24">
         <f>I9 + 1</f>
         <v>11</v>
@@ -1908,8 +1906,8 @@
       </c>
     </row>
     <row r="12" spans="1:13" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="91"/>
-      <c r="B12" s="109"/>
+      <c r="A12" s="92"/>
+      <c r="B12" s="106"/>
       <c r="C12" s="62" t="s">
         <v>54</v>
       </c>
@@ -1927,10 +1925,10 @@
       <c r="I12" s="19"/>
     </row>
     <row r="13" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="91">
+      <c r="A13" s="92">
         <v>11</v>
       </c>
-      <c r="B13" s="109"/>
+      <c r="B13" s="106"/>
       <c r="C13" s="24">
         <f>I11 + 1</f>
         <v>18</v>
@@ -1961,8 +1959,8 @@
       </c>
     </row>
     <row r="14" spans="1:13" ht="83.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="91"/>
-      <c r="B14" s="109"/>
+      <c r="A14" s="92"/>
+      <c r="B14" s="106"/>
       <c r="C14" s="24"/>
       <c r="D14" s="18" t="s">
         <v>28</v>
@@ -1982,10 +1980,10 @@
       <c r="M14" s="42"/>
     </row>
     <row r="15" spans="1:13" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="91">
+      <c r="A15" s="92">
         <v>10</v>
       </c>
-      <c r="B15" s="109"/>
+      <c r="B15" s="106"/>
       <c r="C15" s="63">
         <f>I13 + 1</f>
         <v>25</v>
@@ -2015,8 +2013,8 @@
       </c>
     </row>
     <row r="16" spans="1:13" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="92"/>
-      <c r="B16" s="110"/>
+      <c r="A16" s="93"/>
+      <c r="B16" s="107"/>
       <c r="C16" s="70" t="s">
         <v>41</v>
       </c>
@@ -2163,19 +2161,19 @@
       <c r="I26" s="38"/>
     </row>
     <row r="27" spans="1:11" s="36" customFormat="1" ht="57.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="95" t="str">
+      <c r="A27" s="94" t="str">
         <f>A1</f>
         <v>CS320: SW Engineering - Spring 2018 Schedule
-(as of 4-6-2018, subject to change)</v>
-      </c>
-      <c r="B27" s="96"/>
-      <c r="C27" s="96"/>
-      <c r="D27" s="96"/>
-      <c r="E27" s="96"/>
-      <c r="F27" s="96"/>
-      <c r="G27" s="96"/>
-      <c r="H27" s="96"/>
-      <c r="I27" s="97"/>
+(as of 4-9-2018, subject to change)</v>
+      </c>
+      <c r="B27" s="95"/>
+      <c r="C27" s="95"/>
+      <c r="D27" s="95"/>
+      <c r="E27" s="95"/>
+      <c r="F27" s="95"/>
+      <c r="G27" s="95"/>
+      <c r="H27" s="95"/>
+      <c r="I27" s="96"/>
     </row>
     <row r="28" spans="1:11" s="2" customFormat="1" ht="17.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="str">
@@ -2216,10 +2214,10 @@
       </c>
     </row>
     <row r="29" spans="1:11" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="104">
+      <c r="A29" s="97">
         <v>10</v>
       </c>
-      <c r="B29" s="105" t="s">
+      <c r="B29" s="100" t="s">
         <v>43</v>
       </c>
       <c r="C29" s="63">
@@ -2251,8 +2249,8 @@
       </c>
     </row>
     <row r="30" spans="1:11" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="94"/>
-      <c r="B30" s="106"/>
+      <c r="A30" s="98"/>
+      <c r="B30" s="101"/>
       <c r="C30" s="76" t="s">
         <v>41</v>
       </c>
@@ -2282,10 +2280,10 @@
       </c>
     </row>
     <row r="31" spans="1:11" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="98">
+      <c r="A31" s="99">
         <v>9</v>
       </c>
-      <c r="B31" s="99" t="s">
+      <c r="B31" s="102" t="s">
         <v>15</v>
       </c>
       <c r="C31" s="63">
@@ -2318,8 +2316,8 @@
       </c>
     </row>
     <row r="32" spans="1:11" ht="86.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="91"/>
-      <c r="B32" s="107"/>
+      <c r="A32" s="92"/>
+      <c r="B32" s="103"/>
       <c r="C32" s="63" t="str">
         <f>I30</f>
         <v>WINTER BREAK</v>
@@ -2343,10 +2341,10 @@
       <c r="K32" s="43"/>
     </row>
     <row r="33" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="91">
+      <c r="A33" s="92">
         <v>8</v>
       </c>
-      <c r="B33" s="107"/>
+      <c r="B33" s="103"/>
       <c r="C33" s="28">
         <f>I31 + 1</f>
         <v>11</v>
@@ -2377,8 +2375,8 @@
       </c>
     </row>
     <row r="34" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="91"/>
-      <c r="B34" s="107"/>
+      <c r="A34" s="92"/>
+      <c r="B34" s="103"/>
       <c r="C34" s="10"/>
       <c r="D34" s="44" t="s">
         <v>55</v>
@@ -2397,10 +2395,10 @@
       <c r="K34" s="41"/>
     </row>
     <row r="35" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="91">
+      <c r="A35" s="92">
         <v>7</v>
       </c>
-      <c r="B35" s="107"/>
+      <c r="B35" s="103"/>
       <c r="C35" s="10">
         <f>I33 + 1</f>
         <v>18</v>
@@ -2431,8 +2429,8 @@
       </c>
     </row>
     <row r="36" spans="1:11" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="91"/>
-      <c r="B36" s="107"/>
+      <c r="A36" s="92"/>
+      <c r="B36" s="103"/>
       <c r="C36" s="10"/>
       <c r="D36" s="32" t="s">
         <v>18</v>
@@ -2448,10 +2446,10 @@
       <c r="I36" s="11"/>
     </row>
     <row r="37" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="91">
+      <c r="A37" s="92">
         <v>6</v>
       </c>
-      <c r="B37" s="107"/>
+      <c r="B37" s="103"/>
       <c r="C37" s="10">
         <f>I35 + 1</f>
         <v>25</v>
@@ -2482,8 +2480,8 @@
       </c>
     </row>
     <row r="38" spans="1:11" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="92"/>
-      <c r="B38" s="100"/>
+      <c r="A38" s="93"/>
+      <c r="B38" s="104"/>
       <c r="C38" s="29"/>
       <c r="D38" s="14" t="s">
         <v>19</v>
@@ -2503,10 +2501,10 @@
       </c>
     </row>
     <row r="39" spans="1:11" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="98">
+      <c r="A39" s="99">
         <v>5</v>
       </c>
-      <c r="B39" s="101" t="s">
+      <c r="B39" s="109" t="s">
         <v>16</v>
       </c>
       <c r="C39" s="63">
@@ -2538,8 +2536,8 @@
       </c>
     </row>
     <row r="40" spans="1:11" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="91"/>
-      <c r="B40" s="102"/>
+      <c r="A40" s="92"/>
+      <c r="B40" s="110"/>
       <c r="C40" s="63" t="s">
         <v>6</v>
       </c>
@@ -2554,13 +2552,13 @@
       <c r="H40" s="86" t="s">
         <v>51</v>
       </c>
-      <c r="I40" s="111"/>
+      <c r="I40" s="91"/>
     </row>
     <row r="41" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="91">
+      <c r="A41" s="92">
         <v>4</v>
       </c>
-      <c r="B41" s="102"/>
+      <c r="B41" s="110"/>
       <c r="C41" s="24">
         <f>I39 + 1</f>
         <v>8</v>
@@ -2591,12 +2589,12 @@
       </c>
     </row>
     <row r="42" spans="1:11" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="91"/>
-      <c r="B42" s="102"/>
-      <c r="C42" s="61" t="s">
+      <c r="A42" s="92"/>
+      <c r="B42" s="110"/>
+      <c r="C42" s="62" t="s">
         <v>33</v>
       </c>
-      <c r="D42" s="31" t="s">
+      <c r="D42" s="112" t="s">
         <v>7</v>
       </c>
       <c r="E42" s="17"/>
@@ -2610,10 +2608,10 @@
       <c r="I42" s="53"/>
     </row>
     <row r="43" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="91">
+      <c r="A43" s="92">
         <v>3</v>
       </c>
-      <c r="B43" s="102"/>
+      <c r="B43" s="110"/>
       <c r="C43" s="58">
         <f>I41 + 1</f>
         <v>15</v>
@@ -2644,27 +2642,27 @@
       </c>
     </row>
     <row r="44" spans="1:11" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="91"/>
-      <c r="B44" s="102"/>
+      <c r="A44" s="92"/>
+      <c r="B44" s="110"/>
       <c r="C44" s="56"/>
-      <c r="D44" s="32" t="s">
-        <v>53</v>
+      <c r="D44" s="31" t="s">
+        <v>7</v>
       </c>
       <c r="E44" s="17"/>
       <c r="F44" s="31" t="s">
         <v>7</v>
       </c>
       <c r="G44" s="17"/>
-      <c r="H44" s="31" t="s">
-        <v>7</v>
+      <c r="H44" s="32" t="s">
+        <v>53</v>
       </c>
       <c r="I44" s="19"/>
     </row>
     <row r="45" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="91">
+      <c r="A45" s="92">
         <v>2</v>
       </c>
-      <c r="B45" s="102"/>
+      <c r="B45" s="110"/>
       <c r="C45" s="24">
         <f>I43 + 1</f>
         <v>22</v>
@@ -2695,8 +2693,8 @@
       </c>
     </row>
     <row r="46" spans="1:11" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="91"/>
-      <c r="B46" s="102"/>
+      <c r="A46" s="92"/>
+      <c r="B46" s="110"/>
       <c r="C46" s="23"/>
       <c r="D46" s="44" t="s">
         <v>72</v>
@@ -2714,11 +2712,11 @@
       <c r="I46" s="19"/>
     </row>
     <row r="47" spans="1:11" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="91">
+      <c r="A47" s="92">
         <f>A50 + 1</f>
         <v>1</v>
       </c>
-      <c r="B47" s="102"/>
+      <c r="B47" s="110"/>
       <c r="C47" s="24">
         <f>I45 + 1</f>
         <v>29</v>
@@ -2748,8 +2746,8 @@
       </c>
     </row>
     <row r="48" spans="1:11" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="92"/>
-      <c r="B48" s="103"/>
+      <c r="A48" s="93"/>
+      <c r="B48" s="111"/>
       <c r="C48" s="47"/>
       <c r="D48" s="57" t="s">
         <v>7</v>
@@ -2765,10 +2763,10 @@
       </c>
     </row>
     <row r="49" spans="1:9" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="93">
+      <c r="A49" s="108">
         <v>0</v>
       </c>
-      <c r="B49" s="99" t="s">
+      <c r="B49" s="102" t="s">
         <v>5</v>
       </c>
       <c r="C49" s="10">
@@ -2801,8 +2799,8 @@
       </c>
     </row>
     <row r="50" spans="1:9" ht="129.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="94"/>
-      <c r="B50" s="100"/>
+      <c r="A50" s="98"/>
+      <c r="B50" s="104"/>
       <c r="C50" s="14"/>
       <c r="D50" s="14"/>
       <c r="E50" s="87" t="s">
@@ -2818,6 +2816,18 @@
     <row r="51" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="A47:A48"/>
+    <mergeCell ref="A49:A50"/>
+    <mergeCell ref="A27:I27"/>
+    <mergeCell ref="A33:A34"/>
+    <mergeCell ref="A35:A36"/>
+    <mergeCell ref="A37:A38"/>
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="A41:A42"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="B39:B48"/>
     <mergeCell ref="A13:A14"/>
     <mergeCell ref="A15:A16"/>
     <mergeCell ref="A1:I1"/>
@@ -2832,18 +2842,6 @@
     <mergeCell ref="B31:B38"/>
     <mergeCell ref="B3:B8"/>
     <mergeCell ref="B9:B16"/>
-    <mergeCell ref="A43:A44"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="A47:A48"/>
-    <mergeCell ref="A49:A50"/>
-    <mergeCell ref="A27:I27"/>
-    <mergeCell ref="A33:A34"/>
-    <mergeCell ref="A35:A36"/>
-    <mergeCell ref="A37:A38"/>
-    <mergeCell ref="A39:A40"/>
-    <mergeCell ref="A41:A42"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="B39:B48"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="5" orientation="portrait" r:id="rId1"/>

</xml_diff>